<commit_message>
adds all corrected statement sentences for annotated data
</commit_message>
<xml_diff>
--- a/data/ReferenceErrorDetection_data_annotated.xlsx
+++ b/data/ReferenceErrorDetection_data_annotated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Masterarbeit\citation-verification\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b78b8e360351019/_Dokumente/Studium/Master/Masterarbeit/_citation-verification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3116C6D1-F27C-470A-AF2E-60743673968F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{3116C6D1-F27C-470A-AF2E-60743673968F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A12A4AF5-81B4-4810-A249-BADE86843032}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="6880" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4419" uniqueCount="1860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4456" uniqueCount="1869">
   <si>
     <t>Source</t>
   </si>
@@ -5724,9 +5724,6 @@
     <t>Added</t>
   </si>
   <si>
-    <t>To check whether other tetragonal MAPbX₃ compounds are also pyroelectric, we measured tetragonal MAPbBr₃ well below its phase transition temperature, which is 236.2 K at atmospheric pressure [citation 55], and found no pyroelectric response.</t>
-  </si>
-  <si>
     <t>Wrong number and no mentioning of pressure</t>
   </si>
   <si>
@@ -5829,6 +5826,36 @@
   </si>
   <si>
     <t>Other investigations of Peptide5 in preclinical models have included elucidation of its salutary effects on chronic kidney disease [citation 109].</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>… or a network that is sufficiently sparse that its communities are not detectable [citation 8].</t>
+  </si>
+  <si>
+    <t>This correspondence has been used productively by researchers to … and to explain dependencies between metadata and network structure [citation 35].</t>
+  </si>
+  <si>
+    <t>We reconstituted FUS compartments in vitro at physiological concentration using ... and tested the effect of ATP around its physiological concentration range of ..., complexed with Mg2+ ions (ATP-Mg) [citation 10].</t>
+  </si>
+  <si>
+    <t>…, and the number of S100 positive dendritic cells within the epidermis and dermis was increased in granuloma annulare [citation 13].</t>
+  </si>
+  <si>
+    <t>In early studies, anti-Scl-70 was ..., but, with the use of a more stable antigen, other studies reported the frequency of this antibody to be 75% in this disease [citation 8].</t>
+  </si>
+  <si>
+    <t>This collection included 84% of the high-confidence TFs described by Vaquerizas et al. [citation 23] (classes a and b; table S1)</t>
+  </si>
+  <si>
+    <t>To check whether other tetragonal MAPbX₃ compounds are also pyroelectric, we measured tetragonal MAPbBr₃ (well below its Tc, which equals 236.2 K at atmospheric pressure [citation 55]), and found no pyroelectric response.</t>
+  </si>
+  <si>
+    <t>..., we measured tetragonal MAPbBr3 (well below its Tc, which equals 235 K) [citation 55] and found no pyroelectric response.</t>
+  </si>
+  <si>
+    <t>..., we measured tetragonal MAPbBr₃ (well below its Tc, which equals 236.2 K at atmospheric pressure [citation 55]), and found no pyroelectric response.</t>
   </si>
 </sst>
 </file>
@@ -5890,7 +5917,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -5905,24 +5932,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6227,11 +6240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AE254"/>
+  <dimension ref="A1:X254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6239,9 +6251,8 @@
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="54.85546875" style="5" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="56.85546875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="56.85546875" style="9" customWidth="1"/>
-    <col min="10" max="12" width="25.42578125" style="9" customWidth="1"/>
+    <col min="8" max="9" width="56.85546875" style="5" customWidth="1"/>
+    <col min="10" max="12" width="25.42578125" style="5" customWidth="1"/>
     <col min="14" max="14" width="30.42578125" customWidth="1"/>
     <col min="15" max="15" width="63.85546875" style="5" customWidth="1"/>
     <col min="16" max="16" width="24.5703125" customWidth="1"/>
@@ -6249,13 +6260,12 @@
     <col min="19" max="19" width="12" customWidth="1"/>
     <col min="20" max="20" width="16.28515625" customWidth="1"/>
     <col min="21" max="21" width="21.85546875" customWidth="1"/>
-    <col min="22" max="22" width="18.5703125" style="12" customWidth="1"/>
-    <col min="23" max="23" width="46.28515625" style="12" customWidth="1"/>
-    <col min="24" max="24" width="18.5703125" style="12" customWidth="1"/>
-    <col min="26" max="31" width="9.140625" style="12"/>
+    <col min="22" max="22" width="18.5703125" customWidth="1"/>
+    <col min="23" max="23" width="46.28515625" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6280,16 +6290,16 @@
       <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="7" t="s">
         <v>1828</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="4" t="s">
         <v>1795</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="4" t="s">
         <v>1799</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="4" t="s">
         <v>1800</v>
       </c>
       <c r="M1" s="3" t="s">
@@ -6319,17 +6329,17 @@
       <c r="U1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="3" t="s">
         <v>1796</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="3" t="s">
         <v>1797</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="6" t="s">
         <v>1809</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -6388,14 +6398,8 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
-      <c r="Z2"/>
-      <c r="AA2"/>
-      <c r="AB2"/>
-      <c r="AC2"/>
-      <c r="AD2"/>
-      <c r="AE2"/>
-    </row>
-    <row r="3" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -6454,14 +6458,8 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
-      <c r="Z3"/>
-      <c r="AA3"/>
-      <c r="AB3"/>
-      <c r="AC3"/>
-      <c r="AD3"/>
-      <c r="AE3"/>
-    </row>
-    <row r="4" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -6520,14 +6518,8 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-      <c r="AB4"/>
-      <c r="AC4"/>
-      <c r="AD4"/>
-      <c r="AE4"/>
-    </row>
-    <row r="5" spans="1:31" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -6586,14 +6578,8 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
-      <c r="Z5"/>
-      <c r="AA5"/>
-      <c r="AB5"/>
-      <c r="AC5"/>
-      <c r="AD5"/>
-      <c r="AE5"/>
-    </row>
-    <row r="6" spans="1:31" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -6652,14 +6638,8 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6"/>
-      <c r="AD6"/>
-      <c r="AE6"/>
-    </row>
-    <row r="7" spans="1:31" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -6718,14 +6698,8 @@
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
-      <c r="Z7"/>
-      <c r="AA7"/>
-      <c r="AB7"/>
-      <c r="AC7"/>
-      <c r="AD7"/>
-      <c r="AE7"/>
-    </row>
-    <row r="8" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -6784,14 +6758,8 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
-      <c r="Z8"/>
-      <c r="AA8"/>
-      <c r="AB8"/>
-      <c r="AC8"/>
-      <c r="AD8"/>
-      <c r="AE8"/>
-    </row>
-    <row r="9" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -6850,14 +6818,8 @@
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
-      <c r="Z9"/>
-      <c r="AA9"/>
-      <c r="AB9"/>
-      <c r="AC9"/>
-      <c r="AD9"/>
-      <c r="AE9"/>
-    </row>
-    <row r="10" spans="1:31" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -6916,14 +6878,8 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
-      <c r="Z10"/>
-      <c r="AA10"/>
-      <c r="AB10"/>
-      <c r="AC10"/>
-      <c r="AD10"/>
-      <c r="AE10"/>
-    </row>
-    <row r="11" spans="1:31" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -6982,14 +6938,8 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Z11"/>
-      <c r="AA11"/>
-      <c r="AB11"/>
-      <c r="AC11"/>
-      <c r="AD11"/>
-      <c r="AE11"/>
-    </row>
-    <row r="12" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -7048,14 +6998,8 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Z12"/>
-      <c r="AA12"/>
-      <c r="AB12"/>
-      <c r="AC12"/>
-      <c r="AD12"/>
-      <c r="AE12"/>
-    </row>
-    <row r="13" spans="1:31" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -7114,14 +7058,8 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
-      <c r="Z13"/>
-      <c r="AA13"/>
-      <c r="AB13"/>
-      <c r="AC13"/>
-      <c r="AD13"/>
-      <c r="AE13"/>
-    </row>
-    <row r="14" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -7180,14 +7118,8 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
-      <c r="Z14"/>
-      <c r="AA14"/>
-      <c r="AB14"/>
-      <c r="AC14"/>
-      <c r="AD14"/>
-      <c r="AE14"/>
-    </row>
-    <row r="15" spans="1:31" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -7246,14 +7178,8 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
-      <c r="Z15"/>
-      <c r="AA15"/>
-      <c r="AB15"/>
-      <c r="AC15"/>
-      <c r="AD15"/>
-      <c r="AE15"/>
-    </row>
-    <row r="16" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -7312,14 +7238,8 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
-      <c r="Z16"/>
-      <c r="AA16"/>
-      <c r="AB16"/>
-      <c r="AC16"/>
-      <c r="AD16"/>
-      <c r="AE16"/>
-    </row>
-    <row r="17" spans="1:24" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -7379,7 +7299,7 @@
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
     </row>
-    <row r="18" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -7439,7 +7359,7 @@
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
     </row>
-    <row r="19" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -7499,7 +7419,7 @@
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
     </row>
-    <row r="20" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -7559,7 +7479,7 @@
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
     </row>
-    <row r="21" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -7619,7 +7539,7 @@
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
     </row>
-    <row r="22" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -7679,7 +7599,7 @@
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
     </row>
-    <row r="23" spans="1:24" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -7739,7 +7659,7 @@
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
     </row>
-    <row r="24" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -7799,7 +7719,7 @@
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
     </row>
-    <row r="25" spans="1:24" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -7859,7 +7779,7 @@
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
     </row>
-    <row r="26" spans="1:24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
@@ -7884,7 +7804,9 @@
       <c r="H26" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="I26" s="2"/>
+      <c r="I26" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J26" s="2" t="s">
         <v>1798</v>
       </c>
@@ -7929,7 +7851,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:24" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
@@ -7989,7 +7911,7 @@
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
     </row>
-    <row r="28" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
@@ -8049,7 +7971,7 @@
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
     </row>
-    <row r="29" spans="1:24" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
@@ -8074,7 +7996,9 @@
       <c r="H29" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="I29" s="2"/>
+      <c r="I29" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J29" s="2" t="s">
         <v>1803</v>
       </c>
@@ -8119,7 +8043,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
@@ -8144,7 +8068,9 @@
       <c r="H30" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="I30" s="2"/>
+      <c r="I30" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J30" s="2" t="s">
         <v>1805</v>
       </c>
@@ -8189,7 +8115,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
@@ -8255,7 +8181,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
@@ -8280,7 +8206,9 @@
       <c r="H32" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="I32" s="2"/>
+      <c r="I32" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J32" s="2" t="s">
         <v>1805</v>
       </c>
@@ -8325,7 +8253,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
@@ -8385,7 +8313,7 @@
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
     </row>
-    <row r="34" spans="1:28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -8445,7 +8373,7 @@
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
     </row>
-    <row r="35" spans="1:28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
@@ -8505,7 +8433,7 @@
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
     </row>
-    <row r="36" spans="1:28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>17</v>
       </c>
@@ -8565,7 +8493,7 @@
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
     </row>
-    <row r="37" spans="1:28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -8625,7 +8553,7 @@
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
     </row>
-    <row r="38" spans="1:28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>17</v>
       </c>
@@ -8685,7 +8613,7 @@
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
     </row>
-    <row r="39" spans="1:28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>17</v>
       </c>
@@ -8745,7 +8673,7 @@
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
     </row>
-    <row r="40" spans="1:28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -8805,7 +8733,7 @@
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
     </row>
-    <row r="41" spans="1:28" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -8865,7 +8793,7 @@
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
     </row>
-    <row r="42" spans="1:28" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
@@ -8925,7 +8853,7 @@
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
     </row>
-    <row r="43" spans="1:28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
@@ -8985,7 +8913,7 @@
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
     </row>
-    <row r="44" spans="1:28" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>17</v>
       </c>
@@ -9045,7 +8973,7 @@
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
     </row>
-    <row r="45" spans="1:28" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>17</v>
       </c>
@@ -9105,7 +9033,7 @@
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
     </row>
-    <row r="46" spans="1:28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
@@ -9165,7 +9093,7 @@
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
     </row>
-    <row r="47" spans="1:28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>17</v>
       </c>
@@ -9225,7 +9153,7 @@
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
     </row>
-    <row r="48" spans="1:28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>17</v>
       </c>
@@ -9250,14 +9178,16 @@
       <c r="H48" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7" t="s">
+      <c r="I48" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J48" s="2" t="s">
         <v>1820</v>
       </c>
-      <c r="K48" s="7" t="s">
+      <c r="K48" s="2" t="s">
         <v>1798</v>
       </c>
-      <c r="L48" s="7" t="s">
+      <c r="L48" s="2" t="s">
         <v>1811</v>
       </c>
       <c r="M48" s="1" t="s">
@@ -9287,18 +9217,15 @@
       <c r="U48" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="V48" s="6" t="s">
+      <c r="V48" s="1" t="s">
         <v>1802</v>
       </c>
-      <c r="W48" s="6"/>
-      <c r="X48" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z48" s="12"/>
-      <c r="AA48" s="12"/>
-      <c r="AB48" s="12"/>
-    </row>
-    <row r="49" spans="1:28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="W48" s="1"/>
+      <c r="X48" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>17</v>
       </c>
@@ -9323,14 +9250,16 @@
       <c r="H49" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7" t="s">
+      <c r="I49" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J49" s="2" t="s">
         <v>1820</v>
       </c>
-      <c r="K49" s="7" t="s">
+      <c r="K49" s="2" t="s">
         <v>1798</v>
       </c>
-      <c r="L49" s="7" t="s">
+      <c r="L49" s="2" t="s">
         <v>1811</v>
       </c>
       <c r="M49" s="1" t="s">
@@ -9360,18 +9289,15 @@
       <c r="U49" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="V49" s="6" t="s">
+      <c r="V49" s="1" t="s">
         <v>1802</v>
       </c>
-      <c r="W49" s="6"/>
-      <c r="X49" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z49" s="12"/>
-      <c r="AA49" s="12"/>
-      <c r="AB49" s="12"/>
-    </row>
-    <row r="50" spans="1:28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="W49" s="1"/>
+      <c r="X49" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>17</v>
       </c>
@@ -9431,7 +9357,7 @@
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
     </row>
-    <row r="51" spans="1:28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>17</v>
       </c>
@@ -9491,7 +9417,7 @@
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
     </row>
-    <row r="52" spans="1:28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>17</v>
       </c>
@@ -9551,7 +9477,7 @@
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
     </row>
-    <row r="53" spans="1:28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>17</v>
       </c>
@@ -9611,7 +9537,7 @@
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
     </row>
-    <row r="54" spans="1:28" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>17</v>
       </c>
@@ -9636,14 +9562,16 @@
       <c r="H54" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7" t="s">
+      <c r="I54" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J54" s="2" t="s">
         <v>1820</v>
       </c>
-      <c r="K54" s="7" t="s">
+      <c r="K54" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L54" s="7" t="s">
+      <c r="L54" s="2" t="s">
         <v>1804</v>
       </c>
       <c r="M54" s="1" t="s">
@@ -9671,20 +9599,17 @@
         <v>29</v>
       </c>
       <c r="U54" s="1" t="s">
-        <v>1848</v>
-      </c>
-      <c r="V54" s="6" t="s">
+        <v>1847</v>
+      </c>
+      <c r="V54" s="1" t="s">
         <v>1821</v>
       </c>
-      <c r="W54" s="6"/>
-      <c r="X54" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z54" s="12"/>
-      <c r="AA54" s="12"/>
-      <c r="AB54" s="12"/>
-    </row>
-    <row r="55" spans="1:28" customFormat="1" ht="315" hidden="1" x14ac:dyDescent="0.25">
+      <c r="W54" s="1"/>
+      <c r="X54" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" ht="315" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>17</v>
       </c>
@@ -9707,16 +9632,18 @@
         <v>324</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>1849</v>
-      </c>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7" t="s">
+        <v>1848</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J55" s="2" t="s">
         <v>1820</v>
       </c>
-      <c r="K55" s="7" t="s">
+      <c r="K55" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L55" s="7" t="s">
+      <c r="L55" s="2" t="s">
         <v>1804</v>
       </c>
       <c r="M55" s="1" t="s">
@@ -9744,18 +9671,15 @@
         <v>673</v>
       </c>
       <c r="U55" s="1"/>
-      <c r="V55" s="6"/>
-      <c r="W55" s="7" t="s">
-        <v>1850</v>
-      </c>
-      <c r="X55" s="6" t="s">
+      <c r="V55" s="1"/>
+      <c r="W55" s="2" t="s">
+        <v>1849</v>
+      </c>
+      <c r="X55" s="1" t="s">
         <v>1835</v>
       </c>
-      <c r="Z55" s="12"/>
-      <c r="AA55" s="12"/>
-      <c r="AB55" s="12"/>
-    </row>
-    <row r="56" spans="1:28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>17</v>
       </c>
@@ -9815,7 +9739,7 @@
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
     </row>
-    <row r="57" spans="1:28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>17</v>
       </c>
@@ -9875,7 +9799,7 @@
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
     </row>
-    <row r="58" spans="1:28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>17</v>
       </c>
@@ -9935,7 +9859,7 @@
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
     </row>
-    <row r="59" spans="1:28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>17</v>
       </c>
@@ -9995,7 +9919,7 @@
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
     </row>
-    <row r="60" spans="1:28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>17</v>
       </c>
@@ -10055,7 +9979,7 @@
       <c r="W60" s="1"/>
       <c r="X60" s="1"/>
     </row>
-    <row r="61" spans="1:28" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>17</v>
       </c>
@@ -10115,7 +10039,7 @@
       <c r="W61" s="1"/>
       <c r="X61" s="1"/>
     </row>
-    <row r="62" spans="1:28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>17</v>
       </c>
@@ -10175,7 +10099,7 @@
       <c r="W62" s="1"/>
       <c r="X62" s="1"/>
     </row>
-    <row r="63" spans="1:28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>17</v>
       </c>
@@ -10235,7 +10159,7 @@
       <c r="W63" s="1"/>
       <c r="X63" s="1"/>
     </row>
-    <row r="64" spans="1:28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>17</v>
       </c>
@@ -10295,7 +10219,7 @@
       <c r="W64" s="1"/>
       <c r="X64" s="1"/>
     </row>
-    <row r="65" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>17</v>
       </c>
@@ -10355,7 +10279,7 @@
       <c r="W65" s="1"/>
       <c r="X65" s="1"/>
     </row>
-    <row r="66" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>17</v>
       </c>
@@ -10415,7 +10339,7 @@
       <c r="W66" s="1"/>
       <c r="X66" s="1"/>
     </row>
-    <row r="67" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>17</v>
       </c>
@@ -10475,7 +10399,7 @@
       <c r="W67" s="1"/>
       <c r="X67" s="1"/>
     </row>
-    <row r="68" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>17</v>
       </c>
@@ -10535,7 +10459,7 @@
       <c r="W68" s="1"/>
       <c r="X68" s="1"/>
     </row>
-    <row r="69" spans="1:24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>17</v>
       </c>
@@ -10560,7 +10484,9 @@
       <c r="H69" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="I69" s="2"/>
+      <c r="I69" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J69" s="2" t="s">
         <v>1810</v>
       </c>
@@ -10605,7 +10531,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>17</v>
       </c>
@@ -10630,7 +10556,9 @@
       <c r="H70" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="I70" s="2"/>
+      <c r="I70" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J70" s="2" t="s">
         <v>1810</v>
       </c>
@@ -10675,7 +10603,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>17</v>
       </c>
@@ -10700,7 +10628,9 @@
       <c r="H71" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="I71" s="2"/>
+      <c r="I71" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J71" s="2" t="s">
         <v>1810</v>
       </c>
@@ -10745,7 +10675,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:24" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>17</v>
       </c>
@@ -10770,7 +10700,9 @@
       <c r="H72" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="I72" s="2"/>
+      <c r="I72" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J72" s="2" t="s">
         <v>1810</v>
       </c>
@@ -10815,7 +10747,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:24" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>17</v>
       </c>
@@ -10840,7 +10772,9 @@
       <c r="H73" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="I73" s="2"/>
+      <c r="I73" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J73" s="2" t="s">
         <v>1803</v>
       </c>
@@ -10885,7 +10819,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:24" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>17</v>
       </c>
@@ -10910,7 +10844,9 @@
       <c r="H74" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="I74" s="2"/>
+      <c r="I74" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J74" s="2" t="s">
         <v>1803</v>
       </c>
@@ -10955,7 +10891,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>17</v>
       </c>
@@ -11015,7 +10951,7 @@
       <c r="W75" s="1"/>
       <c r="X75" s="1"/>
     </row>
-    <row r="76" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>17</v>
       </c>
@@ -11075,7 +11011,7 @@
       <c r="W76" s="1"/>
       <c r="X76" s="1"/>
     </row>
-    <row r="77" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>17</v>
       </c>
@@ -11133,7 +11069,7 @@
       <c r="W77" s="1"/>
       <c r="X77" s="1"/>
     </row>
-    <row r="78" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>17</v>
       </c>
@@ -11193,7 +11129,7 @@
       <c r="W78" s="1"/>
       <c r="X78" s="1"/>
     </row>
-    <row r="79" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>17</v>
       </c>
@@ -11253,7 +11189,7 @@
       <c r="W79" s="1"/>
       <c r="X79" s="1"/>
     </row>
-    <row r="80" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -11313,7 +11249,7 @@
       <c r="W80" s="1"/>
       <c r="X80" s="1"/>
     </row>
-    <row r="81" spans="1:29" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>17</v>
       </c>
@@ -11373,7 +11309,7 @@
       <c r="W81" s="1"/>
       <c r="X81" s="1"/>
     </row>
-    <row r="82" spans="1:29" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>17</v>
       </c>
@@ -11433,69 +11369,69 @@
       <c r="W82" s="1"/>
       <c r="X82" s="1"/>
     </row>
-    <row r="83" spans="1:29" s="12" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="6" t="s">
+    <row r="83" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B83" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="D83" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="E83" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G83" s="6" t="s">
+      <c r="E83" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="H83" s="7" t="s">
+      <c r="H83" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="I83" s="7"/>
-      <c r="J83" s="7"/>
-      <c r="K83" s="7"/>
-      <c r="L83" s="7"/>
-      <c r="M83" s="6" t="s">
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
+      <c r="L83" s="2"/>
+      <c r="M83" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="N83" s="6" t="s">
+      <c r="N83" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="O83" s="7" t="s">
+      <c r="O83" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="P83" s="6" t="s">
+      <c r="P83" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="Q83" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R83" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="S83" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="T83" s="6" t="s">
+      <c r="Q83" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R83" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S83" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T83" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U83" s="6" t="s">
+      <c r="U83" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="V83" s="6"/>
-      <c r="W83" s="6"/>
-      <c r="X83" s="6" t="s">
-        <v>1851</v>
-      </c>
-    </row>
-    <row r="84" spans="1:29" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V83" s="1"/>
+      <c r="W83" s="1"/>
+      <c r="X83" s="1" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24" ht="300" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>637</v>
       </c>
@@ -11518,16 +11454,18 @@
         <v>324</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>1853</v>
-      </c>
-      <c r="I84" s="7"/>
-      <c r="J84" s="7" t="s">
+        <v>1852</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J84" s="2" t="s">
         <v>1803</v>
       </c>
-      <c r="K84" s="7" t="s">
+      <c r="K84" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L84" s="7" t="s">
+      <c r="L84" s="2" t="s">
         <v>1812</v>
       </c>
       <c r="M84" s="1" t="s">
@@ -11555,17 +11493,15 @@
         <v>673</v>
       </c>
       <c r="U84" s="1"/>
-      <c r="V84" s="6"/>
-      <c r="W84" s="7" t="s">
-        <v>1852</v>
-      </c>
-      <c r="X84" s="6" t="s">
+      <c r="V84" s="1"/>
+      <c r="W84" s="2" t="s">
+        <v>1851</v>
+      </c>
+      <c r="X84" s="1" t="s">
         <v>1835</v>
       </c>
-      <c r="Z84" s="12"/>
-      <c r="AA84" s="12"/>
-    </row>
-    <row r="85" spans="1:29" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:24" ht="300" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>637</v>
       </c>
@@ -11590,14 +11526,16 @@
       <c r="H85" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="I85" s="7"/>
-      <c r="J85" s="7" t="s">
+      <c r="I85" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J85" s="2" t="s">
         <v>1803</v>
       </c>
-      <c r="K85" s="7" t="s">
+      <c r="K85" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L85" s="7" t="s">
+      <c r="L85" s="2" t="s">
         <v>1812</v>
       </c>
       <c r="M85" s="1" t="s">
@@ -11627,19 +11565,17 @@
       <c r="U85" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="V85" s="6" t="s">
+      <c r="V85" s="1" t="s">
         <v>1821</v>
       </c>
-      <c r="W85" s="7" t="s">
-        <v>1852</v>
-      </c>
-      <c r="X85" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z85" s="12"/>
-      <c r="AA85" s="12"/>
-    </row>
-    <row r="86" spans="1:29" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="W85" s="2" t="s">
+        <v>1851</v>
+      </c>
+      <c r="X85" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>637</v>
       </c>
@@ -11664,15 +11600,17 @@
       <c r="H86" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="I86" s="7"/>
-      <c r="J86" s="7" t="s">
+      <c r="I86" s="2" t="s">
+        <v>1862</v>
+      </c>
+      <c r="J86" s="2" t="s">
         <v>1805</v>
       </c>
-      <c r="K86" s="7" t="s">
+      <c r="K86" s="2" t="s">
         <v>1806</v>
       </c>
-      <c r="L86" s="7" t="s">
-        <v>1854</v>
+      <c r="L86" s="2" t="s">
+        <v>1853</v>
       </c>
       <c r="M86" s="1" t="s">
         <v>678</v>
@@ -11701,15 +11639,13 @@
       <c r="U86" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="V86" s="6"/>
-      <c r="W86" s="6"/>
-      <c r="X86" s="6" t="s">
+      <c r="V86" s="1"/>
+      <c r="W86" s="1"/>
+      <c r="X86" s="1" t="s">
         <v>1825</v>
       </c>
-      <c r="Z86" s="12"/>
-      <c r="AA86" s="12"/>
-    </row>
-    <row r="87" spans="1:29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>637</v>
       </c>
@@ -11734,14 +11670,16 @@
       <c r="H87" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="I87" s="7"/>
-      <c r="J87" s="7" t="s">
+      <c r="I87" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J87" s="2" t="s">
         <v>1805</v>
       </c>
-      <c r="K87" s="7" t="s">
+      <c r="K87" s="2" t="s">
         <v>1806</v>
       </c>
-      <c r="L87" s="7" t="s">
+      <c r="L87" s="2" t="s">
         <v>1807</v>
       </c>
       <c r="M87" s="1" t="s">
@@ -11769,19 +11707,17 @@
         <v>29</v>
       </c>
       <c r="U87" s="1" t="s">
-        <v>1855</v>
-      </c>
-      <c r="V87" s="6" t="s">
+        <v>1854</v>
+      </c>
+      <c r="V87" s="1" t="s">
         <v>1802</v>
       </c>
-      <c r="W87" s="6"/>
-      <c r="X87" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z87" s="12"/>
-      <c r="AA87" s="12"/>
-    </row>
-    <row r="88" spans="1:29" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="W87" s="1"/>
+      <c r="X87" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>637</v>
       </c>
@@ -11806,16 +11742,16 @@
       <c r="H88" s="2" t="s">
         <v>880</v>
       </c>
-      <c r="I88" s="7" t="s">
-        <v>1857</v>
-      </c>
-      <c r="J88" s="7" t="s">
+      <c r="I88" s="2" t="s">
+        <v>1856</v>
+      </c>
+      <c r="J88" s="2" t="s">
         <v>1814</v>
       </c>
-      <c r="K88" s="7" t="s">
+      <c r="K88" s="2" t="s">
         <v>1806</v>
       </c>
-      <c r="L88" s="7" t="s">
+      <c r="L88" s="2" t="s">
         <v>1807</v>
       </c>
       <c r="M88" s="1" t="s">
@@ -11843,19 +11779,17 @@
         <v>29</v>
       </c>
       <c r="U88" s="1" t="s">
-        <v>1856</v>
-      </c>
-      <c r="V88" s="6" t="s">
+        <v>1855</v>
+      </c>
+      <c r="V88" s="1" t="s">
         <v>1821</v>
       </c>
-      <c r="W88" s="6"/>
-      <c r="X88" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z88" s="12"/>
-      <c r="AA88" s="12"/>
-    </row>
-    <row r="89" spans="1:29" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="W88" s="1"/>
+      <c r="X88" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>541</v>
       </c>
@@ -11880,14 +11814,16 @@
       <c r="H89" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="I89" s="7"/>
-      <c r="J89" s="7" t="s">
+      <c r="I89" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J89" s="2" t="s">
         <v>1803</v>
       </c>
-      <c r="K89" s="7" t="s">
+      <c r="K89" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L89" s="7" t="s">
+      <c r="L89" s="2" t="s">
         <v>1804</v>
       </c>
       <c r="M89" s="1" t="s">
@@ -11917,19 +11853,15 @@
       <c r="U89" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="V89" s="6" t="s">
+      <c r="V89" s="1" t="s">
         <v>1808</v>
       </c>
-      <c r="W89" s="6"/>
-      <c r="X89" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z89" s="12"/>
-      <c r="AA89" s="12"/>
-      <c r="AB89" s="12"/>
-      <c r="AC89" s="12"/>
-    </row>
-    <row r="90" spans="1:29" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="W89" s="1"/>
+      <c r="X89" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>541</v>
       </c>
@@ -11955,15 +11887,15 @@
         <v>561</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>1858</v>
-      </c>
-      <c r="J90" s="7" t="s">
+        <v>1857</v>
+      </c>
+      <c r="J90" s="2" t="s">
         <v>1803</v>
       </c>
-      <c r="K90" s="7" t="s">
+      <c r="K90" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L90" s="7" t="s">
+      <c r="L90" s="2" t="s">
         <v>1804</v>
       </c>
       <c r="M90" s="1" t="s">
@@ -11993,19 +11925,15 @@
       <c r="U90" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="V90" s="6" t="s">
+      <c r="V90" s="1" t="s">
         <v>1808</v>
       </c>
-      <c r="W90" s="6"/>
-      <c r="X90" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z90" s="12"/>
-      <c r="AA90" s="12"/>
-      <c r="AB90" s="12"/>
-      <c r="AC90" s="12"/>
-    </row>
-    <row r="91" spans="1:29" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="W90" s="1"/>
+      <c r="X90" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>584</v>
       </c>
@@ -12030,7 +11958,9 @@
       <c r="H91" s="2" t="s">
         <v>1819</v>
       </c>
-      <c r="I91" s="2"/>
+      <c r="I91" s="2" t="s">
+        <v>1863</v>
+      </c>
       <c r="J91" s="2" t="s">
         <v>1820</v>
       </c>
@@ -12075,7 +12005,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:29" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>584</v>
       </c>
@@ -12100,7 +12030,9 @@
       <c r="H92" s="2" t="s">
         <v>1822</v>
       </c>
-      <c r="I92" s="2"/>
+      <c r="I92" s="2" t="s">
+        <v>1864</v>
+      </c>
       <c r="J92" s="2" t="s">
         <v>1803</v>
       </c>
@@ -12145,7 +12077,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:29" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>601</v>
       </c>
@@ -12170,7 +12102,9 @@
       <c r="H93" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="I93" s="2"/>
+      <c r="I93" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J93" s="2" t="s">
         <v>1820</v>
       </c>
@@ -12215,7 +12149,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:29" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>611</v>
       </c>
@@ -12240,12 +12174,14 @@
       <c r="H94" s="2" t="s">
         <v>616</v>
       </c>
-      <c r="I94" s="2"/>
+      <c r="I94" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J94" s="2" t="s">
         <v>1820</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>1824</v>
@@ -12285,7 +12221,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:29" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>621</v>
       </c>
@@ -12343,7 +12279,7 @@
       <c r="W95" s="1"/>
       <c r="X95" s="1"/>
     </row>
-    <row r="96" spans="1:29" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>621</v>
       </c>
@@ -12401,7 +12337,7 @@
       <c r="W96" s="1"/>
       <c r="X96" s="1"/>
     </row>
-    <row r="97" spans="1:31" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>621</v>
       </c>
@@ -12458,14 +12394,8 @@
       <c r="V97" s="1"/>
       <c r="W97" s="1"/>
       <c r="X97" s="1"/>
-      <c r="Z97"/>
-      <c r="AA97"/>
-      <c r="AB97"/>
-      <c r="AC97"/>
-      <c r="AD97"/>
-      <c r="AE97"/>
-    </row>
-    <row r="98" spans="1:31" ht="405" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:24" ht="405" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>637</v>
       </c>
@@ -12490,7 +12420,9 @@
       <c r="H98" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="I98" s="2"/>
+      <c r="I98" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J98" s="2" t="s">
         <v>1798</v>
       </c>
@@ -12534,14 +12466,8 @@
       <c r="X98" s="1" t="s">
         <v>1825</v>
       </c>
-      <c r="Z98"/>
-      <c r="AA98"/>
-      <c r="AB98"/>
-      <c r="AC98"/>
-      <c r="AD98"/>
-      <c r="AE98"/>
-    </row>
-    <row r="99" spans="1:31" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>541</v>
       </c>
@@ -12567,15 +12493,15 @@
         <v>566</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>1859</v>
-      </c>
-      <c r="J99" s="7" t="s">
+        <v>1858</v>
+      </c>
+      <c r="J99" s="2" t="s">
         <v>1803</v>
       </c>
-      <c r="K99" s="7" t="s">
+      <c r="K99" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L99" s="7" t="s">
+      <c r="L99" s="2" t="s">
         <v>1804</v>
       </c>
       <c r="M99" s="1" t="s">
@@ -12605,17 +12531,15 @@
       <c r="U99" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="V99" s="6" t="s">
+      <c r="V99" s="1" t="s">
         <v>1808</v>
       </c>
-      <c r="W99" s="6"/>
-      <c r="X99" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD99"/>
-      <c r="AE99"/>
-    </row>
-    <row r="100" spans="1:31" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="W99" s="1"/>
+      <c r="X99" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>637</v>
       </c>
@@ -12672,14 +12596,8 @@
       <c r="V100" s="1"/>
       <c r="W100" s="1"/>
       <c r="X100" s="1"/>
-      <c r="Z100"/>
-      <c r="AA100"/>
-      <c r="AB100"/>
-      <c r="AC100"/>
-      <c r="AD100"/>
-      <c r="AE100"/>
-    </row>
-    <row r="101" spans="1:31" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>637</v>
       </c>
@@ -12738,84 +12656,80 @@
       <c r="V101" s="1"/>
       <c r="W101" s="1"/>
       <c r="X101" s="1"/>
-      <c r="Z101"/>
-      <c r="AA101"/>
-      <c r="AB101"/>
-      <c r="AC101"/>
-      <c r="AD101"/>
-      <c r="AE101"/>
-    </row>
-    <row r="102" spans="1:31" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="6" t="s">
+    </row>
+    <row r="102" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="B102" s="6" t="s">
+      <c r="B102" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="C102" s="6" t="s">
+      <c r="C102" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="D102" s="7" t="s">
+      <c r="D102" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="E102" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F102" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G102" s="6" t="s">
+      <c r="E102" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G102" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H102" s="7" t="s">
+      <c r="H102" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="I102" s="7"/>
-      <c r="J102" s="7" t="s">
+      <c r="I102" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J102" s="2" t="s">
         <v>1798</v>
       </c>
-      <c r="K102" s="7" t="s">
+      <c r="K102" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L102" s="7" t="s">
+      <c r="L102" s="2" t="s">
         <v>1812</v>
       </c>
-      <c r="M102" s="6" t="s">
+      <c r="M102" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="N102" s="6" t="s">
+      <c r="N102" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="O102" s="7" t="s">
+      <c r="O102" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="P102" s="6" t="s">
+      <c r="P102" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="Q102" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R102" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="S102" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="T102" s="6" t="s">
+      <c r="Q102" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R102" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S102" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T102" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U102" s="6" t="s">
+      <c r="U102" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="V102" s="6" t="s">
+      <c r="V102" s="1" t="s">
         <v>1808</v>
       </c>
-      <c r="W102" s="6"/>
-      <c r="X102" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="103" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="W102" s="1"/>
+      <c r="X102" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>637</v>
       </c>
@@ -12870,14 +12784,8 @@
       <c r="V103" s="1"/>
       <c r="W103" s="1"/>
       <c r="X103" s="1"/>
-      <c r="Z103"/>
-      <c r="AA103"/>
-      <c r="AB103"/>
-      <c r="AC103"/>
-      <c r="AD103"/>
-      <c r="AE103"/>
-    </row>
-    <row r="104" spans="1:31" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>637</v>
       </c>
@@ -12934,14 +12842,8 @@
       <c r="V104" s="1"/>
       <c r="W104" s="1"/>
       <c r="X104" s="1"/>
-      <c r="Z104"/>
-      <c r="AA104"/>
-      <c r="AB104"/>
-      <c r="AC104"/>
-      <c r="AD104"/>
-      <c r="AE104"/>
-    </row>
-    <row r="105" spans="1:31" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>637</v>
       </c>
@@ -13010,25 +12912,19 @@
       <c r="X105" s="1" t="s">
         <v>1825</v>
       </c>
-      <c r="Z105"/>
-      <c r="AA105"/>
-      <c r="AB105"/>
-      <c r="AC105"/>
-      <c r="AD105"/>
-      <c r="AE105"/>
-    </row>
-    <row r="106" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>637</v>
+        <v>541</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>708</v>
+        <v>570</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>709</v>
+        <v>571</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>710</v>
+        <v>572</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>28</v>
@@ -13037,32 +12933,34 @@
         <v>21</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>324</v>
+        <v>48</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>712</v>
-      </c>
-      <c r="I106" s="2"/>
-      <c r="J106" s="7" t="s">
-        <v>1805</v>
-      </c>
-      <c r="K106" s="7" t="s">
-        <v>1806</v>
-      </c>
-      <c r="L106" s="7" t="s">
-        <v>1807</v>
+        <v>578</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J106" s="2" t="s">
+        <v>1798</v>
+      </c>
+      <c r="K106" s="2" t="s">
+        <v>1801</v>
+      </c>
+      <c r="L106" s="2" t="s">
+        <v>1812</v>
       </c>
       <c r="M106" s="1" t="s">
-        <v>711</v>
+        <v>573</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>713</v>
+        <v>575</v>
       </c>
       <c r="O106" s="2" t="s">
-        <v>714</v>
+        <v>576</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>715</v>
+        <v>577</v>
       </c>
       <c r="Q106" s="1" t="s">
         <v>21</v>
@@ -13074,22 +12972,20 @@
         <v>21</v>
       </c>
       <c r="T106" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="U106" s="1"/>
-      <c r="V106" s="6"/>
-      <c r="W106" s="6"/>
-      <c r="X106" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z106"/>
-      <c r="AA106"/>
-      <c r="AB106"/>
-      <c r="AC106"/>
-      <c r="AD106"/>
-      <c r="AE106"/>
-    </row>
-    <row r="107" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="U106" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="V106" s="1" t="s">
+        <v>1808</v>
+      </c>
+      <c r="W106" s="1"/>
+      <c r="X106" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>637</v>
       </c>
@@ -13146,14 +13042,8 @@
       <c r="V107" s="1"/>
       <c r="W107" s="1"/>
       <c r="X107" s="1"/>
-      <c r="Z107"/>
-      <c r="AA107"/>
-      <c r="AB107"/>
-      <c r="AC107"/>
-      <c r="AD107"/>
-      <c r="AE107"/>
-    </row>
-    <row r="108" spans="1:31" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>637</v>
       </c>
@@ -13181,13 +13071,13 @@
       <c r="I108" s="2" t="s">
         <v>1831</v>
       </c>
-      <c r="J108" s="7" t="s">
+      <c r="J108" s="2" t="s">
         <v>1798</v>
       </c>
-      <c r="K108" s="7" t="s">
+      <c r="K108" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L108" s="7" t="s">
+      <c r="L108" s="2" t="s">
         <v>1804</v>
       </c>
       <c r="M108" s="1" t="s">
@@ -13217,21 +13107,15 @@
       <c r="U108" s="1" t="s">
         <v>1832</v>
       </c>
-      <c r="V108" s="6" t="s">
+      <c r="V108" s="1" t="s">
         <v>1821</v>
       </c>
-      <c r="W108" s="6"/>
-      <c r="X108" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z108"/>
-      <c r="AA108"/>
-      <c r="AB108"/>
-      <c r="AC108"/>
-      <c r="AD108"/>
-      <c r="AE108"/>
-    </row>
-    <row r="109" spans="1:31" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="W108" s="1"/>
+      <c r="X108" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>637</v>
       </c>
@@ -13290,14 +13174,8 @@
       <c r="V109" s="1"/>
       <c r="W109" s="1"/>
       <c r="X109" s="1"/>
-      <c r="Z109"/>
-      <c r="AA109"/>
-      <c r="AB109"/>
-      <c r="AC109"/>
-      <c r="AD109"/>
-      <c r="AE109"/>
-    </row>
-    <row r="110" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>637</v>
       </c>
@@ -13354,84 +13232,80 @@
       <c r="V110" s="1"/>
       <c r="W110" s="1"/>
       <c r="X110" s="1"/>
-      <c r="Z110"/>
-      <c r="AA110"/>
-      <c r="AB110"/>
-      <c r="AC110"/>
-      <c r="AD110"/>
-      <c r="AE110"/>
-    </row>
-    <row r="111" spans="1:31" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A111" s="6" t="s">
+    </row>
+    <row r="111" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="B111" s="6" t="s">
+      <c r="B111" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="C111" s="6" t="s">
+      <c r="C111" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="D111" s="7" t="s">
+      <c r="D111" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="E111" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F111" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G111" s="6" t="s">
+      <c r="E111" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H111" s="7" t="s">
-        <v>578</v>
-      </c>
-      <c r="I111" s="7"/>
-      <c r="J111" s="7" t="s">
+      <c r="H111" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J111" s="2" t="s">
         <v>1798</v>
       </c>
-      <c r="K111" s="7" t="s">
+      <c r="K111" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L111" s="7" t="s">
+      <c r="L111" s="2" t="s">
         <v>1812</v>
       </c>
-      <c r="M111" s="6" t="s">
-        <v>573</v>
-      </c>
-      <c r="N111" s="6" t="s">
-        <v>575</v>
-      </c>
-      <c r="O111" s="7" t="s">
-        <v>576</v>
-      </c>
-      <c r="P111" s="6" t="s">
-        <v>577</v>
-      </c>
-      <c r="Q111" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R111" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="S111" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="T111" s="6" t="s">
+      <c r="M111" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="N111" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="O111" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="P111" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="Q111" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R111" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S111" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T111" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U111" s="6" t="s">
+      <c r="U111" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="V111" s="6" t="s">
+      <c r="V111" s="1" t="s">
         <v>1808</v>
       </c>
-      <c r="W111" s="6"/>
-      <c r="X111" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="112" spans="1:31" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="W111" s="1"/>
+      <c r="X111" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="112" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>637</v>
       </c>
@@ -13488,14 +13362,8 @@
       <c r="V112" s="1"/>
       <c r="W112" s="1"/>
       <c r="X112" s="1"/>
-      <c r="Z112"/>
-      <c r="AA112"/>
-      <c r="AB112"/>
-      <c r="AC112"/>
-      <c r="AD112"/>
-      <c r="AE112"/>
-    </row>
-    <row r="113" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>637</v>
       </c>
@@ -13552,14 +13420,8 @@
       <c r="V113" s="1"/>
       <c r="W113" s="1"/>
       <c r="X113" s="1"/>
-      <c r="Z113"/>
-      <c r="AA113"/>
-      <c r="AB113"/>
-      <c r="AC113"/>
-      <c r="AD113"/>
-      <c r="AE113"/>
-    </row>
-    <row r="114" spans="1:31" ht="210" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>637</v>
       </c>
@@ -13587,13 +13449,13 @@
       <c r="I114" s="2" t="s">
         <v>1833</v>
       </c>
-      <c r="J114" s="7" t="s">
+      <c r="J114" s="2" t="s">
         <v>1810</v>
       </c>
-      <c r="K114" s="7" t="s">
+      <c r="K114" s="2" t="s">
         <v>1806</v>
       </c>
-      <c r="L114" s="7" t="s">
+      <c r="L114" s="2" t="s">
         <v>1807</v>
       </c>
       <c r="M114" s="1" t="s">
@@ -13623,21 +13485,15 @@
       <c r="U114" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="V114" s="6"/>
-      <c r="W114" s="7" t="s">
+      <c r="V114" s="1"/>
+      <c r="W114" s="2" t="s">
         <v>1834</v>
       </c>
-      <c r="X114" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z114"/>
-      <c r="AA114"/>
-      <c r="AB114"/>
-      <c r="AC114"/>
-      <c r="AD114"/>
-      <c r="AE114"/>
-    </row>
-    <row r="115" spans="1:31" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X114" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>637</v>
       </c>
@@ -13694,14 +13550,8 @@
       <c r="V115" s="1"/>
       <c r="W115" s="1"/>
       <c r="X115" s="1"/>
-      <c r="Z115"/>
-      <c r="AA115"/>
-      <c r="AB115"/>
-      <c r="AC115"/>
-      <c r="AD115"/>
-      <c r="AE115"/>
-    </row>
-    <row r="116" spans="1:31" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>637</v>
       </c>
@@ -13760,14 +13610,8 @@
       <c r="V116" s="1"/>
       <c r="W116" s="1"/>
       <c r="X116" s="1"/>
-      <c r="Z116"/>
-      <c r="AA116"/>
-      <c r="AB116"/>
-      <c r="AC116"/>
-      <c r="AD116"/>
-      <c r="AE116"/>
-    </row>
-    <row r="117" spans="1:31" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>637</v>
       </c>
@@ -13824,14 +13668,8 @@
       <c r="V117" s="1"/>
       <c r="W117" s="1"/>
       <c r="X117" s="1"/>
-      <c r="Z117"/>
-      <c r="AA117"/>
-      <c r="AB117"/>
-      <c r="AC117"/>
-      <c r="AD117"/>
-      <c r="AE117"/>
-    </row>
-    <row r="118" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>637</v>
       </c>
@@ -13890,14 +13728,8 @@
       <c r="V118" s="1"/>
       <c r="W118" s="1"/>
       <c r="X118" s="1"/>
-      <c r="Z118"/>
-      <c r="AA118"/>
-      <c r="AB118"/>
-      <c r="AC118"/>
-      <c r="AD118"/>
-      <c r="AE118"/>
-    </row>
-    <row r="119" spans="1:31" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>637</v>
       </c>
@@ -13954,14 +13786,8 @@
       <c r="V119" s="1"/>
       <c r="W119" s="1"/>
       <c r="X119" s="1"/>
-      <c r="Z119"/>
-      <c r="AA119"/>
-      <c r="AB119"/>
-      <c r="AC119"/>
-      <c r="AD119"/>
-      <c r="AE119"/>
-    </row>
-    <row r="120" spans="1:31" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>637</v>
       </c>
@@ -14018,14 +13844,8 @@
       <c r="V120" s="1"/>
       <c r="W120" s="1"/>
       <c r="X120" s="1"/>
-      <c r="Z120"/>
-      <c r="AA120"/>
-      <c r="AB120"/>
-      <c r="AC120"/>
-      <c r="AD120"/>
-      <c r="AE120"/>
-    </row>
-    <row r="121" spans="1:31" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>637</v>
       </c>
@@ -14084,14 +13904,8 @@
       <c r="V121" s="1"/>
       <c r="W121" s="1"/>
       <c r="X121" s="1"/>
-      <c r="Z121"/>
-      <c r="AA121"/>
-      <c r="AB121"/>
-      <c r="AC121"/>
-      <c r="AD121"/>
-      <c r="AE121"/>
-    </row>
-    <row r="122" spans="1:31" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>637</v>
       </c>
@@ -14148,14 +13962,8 @@
       <c r="V122" s="1"/>
       <c r="W122" s="1"/>
       <c r="X122" s="1"/>
-      <c r="Z122"/>
-      <c r="AA122"/>
-      <c r="AB122"/>
-      <c r="AC122"/>
-      <c r="AD122"/>
-      <c r="AE122"/>
-    </row>
-    <row r="123" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>637</v>
       </c>
@@ -14212,14 +14020,8 @@
       <c r="V123" s="1"/>
       <c r="W123" s="1"/>
       <c r="X123" s="1"/>
-      <c r="Z123"/>
-      <c r="AA123"/>
-      <c r="AB123"/>
-      <c r="AC123"/>
-      <c r="AD123"/>
-      <c r="AE123"/>
-    </row>
-    <row r="124" spans="1:31" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>637</v>
       </c>
@@ -14278,25 +14080,19 @@
       <c r="V124" s="1"/>
       <c r="W124" s="1"/>
       <c r="X124" s="1"/>
-      <c r="Z124"/>
-      <c r="AA124"/>
-      <c r="AB124"/>
-      <c r="AC124"/>
-      <c r="AD124"/>
-      <c r="AE124"/>
-    </row>
-    <row r="125" spans="1:31" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>637</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>860</v>
+        <v>708</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>861</v>
+        <v>709</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>862</v>
+        <v>710</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>28</v>
@@ -14305,32 +14101,34 @@
         <v>21</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>39</v>
+        <v>324</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>864</v>
-      </c>
-      <c r="I125" s="2"/>
-      <c r="J125" s="7" t="s">
-        <v>1814</v>
-      </c>
-      <c r="K125" s="7" t="s">
-        <v>1801</v>
-      </c>
-      <c r="L125" s="7" t="s">
-        <v>1830</v>
+        <v>712</v>
+      </c>
+      <c r="I125" s="2" t="s">
+        <v>1865</v>
+      </c>
+      <c r="J125" s="2" t="s">
+        <v>1805</v>
+      </c>
+      <c r="K125" s="2" t="s">
+        <v>1806</v>
+      </c>
+      <c r="L125" s="2" t="s">
+        <v>1807</v>
       </c>
       <c r="M125" s="1" t="s">
-        <v>863</v>
+        <v>711</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>865</v>
+        <v>713</v>
       </c>
       <c r="O125" s="2" t="s">
-        <v>866</v>
+        <v>714</v>
       </c>
       <c r="P125" s="1" t="s">
-        <v>867</v>
+        <v>715</v>
       </c>
       <c r="Q125" s="1" t="s">
         <v>21</v>
@@ -14342,26 +14140,16 @@
         <v>21</v>
       </c>
       <c r="T125" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U125" s="1" t="s">
-        <v>1837</v>
-      </c>
-      <c r="V125" s="6" t="s">
-        <v>1823</v>
-      </c>
-      <c r="W125" s="6"/>
-      <c r="X125" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z125"/>
-      <c r="AA125"/>
-      <c r="AB125"/>
-      <c r="AC125"/>
-      <c r="AD125"/>
-      <c r="AE125"/>
-    </row>
-    <row r="126" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+      <c r="U125" s="1"/>
+      <c r="V125" s="1"/>
+      <c r="W125" s="1"/>
+      <c r="X125" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="126" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>637</v>
       </c>
@@ -14420,84 +14208,80 @@
       <c r="V126" s="1"/>
       <c r="W126" s="1"/>
       <c r="X126" s="1"/>
-      <c r="Z126"/>
-      <c r="AA126"/>
-      <c r="AB126"/>
-      <c r="AC126"/>
-      <c r="AD126"/>
-      <c r="AE126"/>
-    </row>
-    <row r="127" spans="1:31" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A127" s="6" t="s">
-        <v>541</v>
-      </c>
-      <c r="B127" s="6" t="s">
-        <v>570</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>571</v>
-      </c>
-      <c r="D127" s="7" t="s">
-        <v>572</v>
-      </c>
-      <c r="E127" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F127" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G127" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H127" s="7" t="s">
-        <v>580</v>
-      </c>
-      <c r="I127" s="7"/>
-      <c r="J127" s="7" t="s">
-        <v>1798</v>
-      </c>
-      <c r="K127" s="7" t="s">
+    </row>
+    <row r="127" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H127" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="I127" s="2" t="s">
+        <v>1867</v>
+      </c>
+      <c r="J127" s="2" t="s">
+        <v>1814</v>
+      </c>
+      <c r="K127" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L127" s="7" t="s">
-        <v>1812</v>
-      </c>
-      <c r="M127" s="6" t="s">
-        <v>579</v>
-      </c>
-      <c r="N127" s="6" t="s">
-        <v>581</v>
-      </c>
-      <c r="O127" s="7" t="s">
-        <v>582</v>
-      </c>
-      <c r="P127" s="6" t="s">
-        <v>583</v>
-      </c>
-      <c r="Q127" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R127" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="S127" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="T127" s="6" t="s">
+      <c r="L127" s="2" t="s">
+        <v>1830</v>
+      </c>
+      <c r="M127" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="N127" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="O127" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="P127" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="Q127" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R127" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S127" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T127" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U127" s="6" t="s">
-        <v>559</v>
-      </c>
-      <c r="V127" s="6" t="s">
-        <v>1808</v>
-      </c>
-      <c r="W127" s="6"/>
-      <c r="X127" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="128" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U127" s="1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="V127" s="1" t="s">
+        <v>1823</v>
+      </c>
+      <c r="W127" s="1"/>
+      <c r="X127" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="128" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>637</v>
       </c>
@@ -14556,14 +14340,8 @@
       <c r="V128" s="1"/>
       <c r="W128" s="1"/>
       <c r="X128" s="1"/>
-      <c r="Z128"/>
-      <c r="AA128"/>
-      <c r="AB128"/>
-      <c r="AC128"/>
-      <c r="AD128"/>
-      <c r="AE128"/>
-    </row>
-    <row r="129" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>637</v>
       </c>
@@ -14586,16 +14364,18 @@
         <v>39</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>1836</v>
-      </c>
-      <c r="I129" s="2"/>
-      <c r="J129" s="7" t="s">
+        <v>1866</v>
+      </c>
+      <c r="I129" s="2" t="s">
+        <v>1868</v>
+      </c>
+      <c r="J129" s="2" t="s">
         <v>1814</v>
       </c>
-      <c r="K129" s="7" t="s">
+      <c r="K129" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L129" s="7" t="s">
+      <c r="L129" s="2" t="s">
         <v>1830</v>
       </c>
       <c r="M129" s="1" t="s">
@@ -14623,15 +14403,15 @@
         <v>673</v>
       </c>
       <c r="U129" s="1"/>
-      <c r="V129" s="6"/>
-      <c r="W129" s="6" t="s">
-        <v>1838</v>
-      </c>
-      <c r="X129" s="6" t="s">
+      <c r="V129" s="1"/>
+      <c r="W129" s="1" t="s">
+        <v>1837</v>
+      </c>
+      <c r="X129" s="1" t="s">
         <v>1835</v>
       </c>
     </row>
-    <row r="130" spans="1:24" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>637</v>
       </c>
@@ -14656,14 +14436,16 @@
       <c r="H130" s="2" t="s">
         <v>893</v>
       </c>
-      <c r="I130" s="2"/>
-      <c r="J130" s="7" t="s">
+      <c r="I130" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J130" s="2" t="s">
         <v>1814</v>
       </c>
-      <c r="K130" s="7" t="s">
+      <c r="K130" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="L130" s="7" t="s">
+      <c r="L130" s="2" t="s">
         <v>1812</v>
       </c>
       <c r="M130" s="1" t="s">
@@ -14691,15 +14473,15 @@
         <v>673</v>
       </c>
       <c r="U130" s="1"/>
-      <c r="V130" s="6"/>
-      <c r="W130" s="7" t="s">
-        <v>1839</v>
-      </c>
-      <c r="X130" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="131" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V130" s="1"/>
+      <c r="W130" s="2" t="s">
+        <v>1838</v>
+      </c>
+      <c r="X130" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="131" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>637</v>
       </c>
@@ -14759,7 +14541,7 @@
       <c r="W131" s="1"/>
       <c r="X131" s="1"/>
     </row>
-    <row r="132" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>637</v>
       </c>
@@ -14785,15 +14567,15 @@
         <v>906</v>
       </c>
       <c r="I132" s="2" t="s">
+        <v>1839</v>
+      </c>
+      <c r="J132" s="2" t="s">
+        <v>1798</v>
+      </c>
+      <c r="K132" s="2" t="s">
         <v>1840</v>
       </c>
-      <c r="J132" s="7" t="s">
-        <v>1798</v>
-      </c>
-      <c r="K132" s="7" t="s">
-        <v>1841</v>
-      </c>
-      <c r="L132" s="7" t="s">
+      <c r="L132" s="2" t="s">
         <v>1817</v>
       </c>
       <c r="M132" s="1" t="s">
@@ -14821,17 +14603,17 @@
         <v>29</v>
       </c>
       <c r="U132" s="1" t="s">
+        <v>1841</v>
+      </c>
+      <c r="V132" s="1" t="s">
         <v>1842</v>
       </c>
-      <c r="V132" s="6" t="s">
-        <v>1843</v>
-      </c>
-      <c r="W132" s="6"/>
-      <c r="X132" s="6" t="s">
+      <c r="W132" s="1"/>
+      <c r="X132" s="1" t="s">
         <v>1825</v>
       </c>
     </row>
-    <row r="133" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>637</v>
       </c>
@@ -14891,7 +14673,7 @@
       <c r="W133" s="1"/>
       <c r="X133" s="1"/>
     </row>
-    <row r="134" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>637</v>
       </c>
@@ -14951,7 +14733,7 @@
       <c r="W134" s="1"/>
       <c r="X134" s="1"/>
     </row>
-    <row r="135" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>637</v>
       </c>
@@ -14977,16 +14759,16 @@
         <v>930</v>
       </c>
       <c r="I135" s="2" t="s">
+        <v>1843</v>
+      </c>
+      <c r="J135" s="2" t="s">
+        <v>1798</v>
+      </c>
+      <c r="K135" s="2" t="s">
+        <v>1840</v>
+      </c>
+      <c r="L135" s="2" t="s">
         <v>1844</v>
-      </c>
-      <c r="J135" s="7" t="s">
-        <v>1798</v>
-      </c>
-      <c r="K135" s="7" t="s">
-        <v>1841</v>
-      </c>
-      <c r="L135" s="7" t="s">
-        <v>1845</v>
       </c>
       <c r="M135" s="1" t="s">
         <v>929</v>
@@ -15013,17 +14795,17 @@
         <v>29</v>
       </c>
       <c r="U135" s="1" t="s">
-        <v>1846</v>
-      </c>
-      <c r="V135" s="6" t="s">
+        <v>1845</v>
+      </c>
+      <c r="V135" s="1" t="s">
         <v>1802</v>
       </c>
-      <c r="W135" s="6"/>
-      <c r="X135" s="6" t="s">
+      <c r="W135" s="1"/>
+      <c r="X135" s="1" t="s">
         <v>1825</v>
       </c>
     </row>
-    <row r="136" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>637</v>
       </c>
@@ -15081,7 +14863,7 @@
       <c r="W136" s="1"/>
       <c r="X136" s="1"/>
     </row>
-    <row r="137" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>637</v>
       </c>
@@ -15139,7 +14921,7 @@
       <c r="W137" s="1"/>
       <c r="X137" s="1"/>
     </row>
-    <row r="138" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>637</v>
       </c>
@@ -15197,7 +14979,7 @@
       <c r="W138" s="1"/>
       <c r="X138" s="1"/>
     </row>
-    <row r="139" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>637</v>
       </c>
@@ -15255,7 +15037,7 @@
       <c r="W139" s="1"/>
       <c r="X139" s="1"/>
     </row>
-    <row r="140" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>637</v>
       </c>
@@ -15313,7 +15095,7 @@
       <c r="W140" s="1"/>
       <c r="X140" s="1"/>
     </row>
-    <row r="141" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>637</v>
       </c>
@@ -15373,7 +15155,7 @@
       <c r="W141" s="1"/>
       <c r="X141" s="1"/>
     </row>
-    <row r="142" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>637</v>
       </c>
@@ -15431,7 +15213,7 @@
       <c r="W142" s="1"/>
       <c r="X142" s="1"/>
     </row>
-    <row r="143" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>637</v>
       </c>
@@ -15491,7 +15273,7 @@
       <c r="W143" s="1"/>
       <c r="X143" s="1"/>
     </row>
-    <row r="144" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>637</v>
       </c>
@@ -15551,7 +15333,7 @@
       <c r="W144" s="1"/>
       <c r="X144" s="1"/>
     </row>
-    <row r="145" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>637</v>
       </c>
@@ -15609,7 +15391,7 @@
       <c r="W145" s="1"/>
       <c r="X145" s="1"/>
     </row>
-    <row r="146" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>637</v>
       </c>
@@ -15669,7 +15451,7 @@
       <c r="W146" s="1"/>
       <c r="X146" s="1"/>
     </row>
-    <row r="147" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>637</v>
       </c>
@@ -15727,7 +15509,7 @@
       <c r="W147" s="1"/>
       <c r="X147" s="1"/>
     </row>
-    <row r="148" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>637</v>
       </c>
@@ -15787,7 +15569,7 @@
       <c r="W148" s="1"/>
       <c r="X148" s="1"/>
     </row>
-    <row r="149" spans="1:24" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:24" ht="225" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>637</v>
       </c>
@@ -15812,14 +15594,16 @@
       <c r="H149" s="2" t="s">
         <v>1039</v>
       </c>
-      <c r="I149" s="2"/>
-      <c r="J149" s="7" t="s">
+      <c r="I149" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J149" s="2" t="s">
         <v>1814</v>
       </c>
-      <c r="K149" s="7" t="s">
-        <v>1841</v>
-      </c>
-      <c r="L149" s="7" t="s">
+      <c r="K149" s="2" t="s">
+        <v>1840</v>
+      </c>
+      <c r="L149" s="2" t="s">
         <v>1824</v>
       </c>
       <c r="M149" s="1" t="s">
@@ -15847,15 +15631,15 @@
         <v>673</v>
       </c>
       <c r="U149" s="1"/>
-      <c r="V149" s="6"/>
-      <c r="W149" s="7" t="s">
-        <v>1847</v>
-      </c>
-      <c r="X149" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="150" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V149" s="1"/>
+      <c r="W149" s="2" t="s">
+        <v>1846</v>
+      </c>
+      <c r="X149" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="150" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>637</v>
       </c>
@@ -15915,7 +15699,7 @@
       <c r="W150" s="1"/>
       <c r="X150" s="1"/>
     </row>
-    <row r="151" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>637</v>
       </c>
@@ -15975,7 +15759,7 @@
       <c r="W151" s="1"/>
       <c r="X151" s="1"/>
     </row>
-    <row r="152" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>637</v>
       </c>
@@ -16035,7 +15819,7 @@
       <c r="W152" s="1"/>
       <c r="X152" s="1"/>
     </row>
-    <row r="153" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>637</v>
       </c>
@@ -16093,7 +15877,7 @@
       <c r="W153" s="1"/>
       <c r="X153" s="1"/>
     </row>
-    <row r="154" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>637</v>
       </c>
@@ -16153,7 +15937,7 @@
       <c r="W154" s="1"/>
       <c r="X154" s="1"/>
     </row>
-    <row r="155" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>637</v>
       </c>
@@ -16211,7 +15995,7 @@
       <c r="W155" s="1"/>
       <c r="X155" s="1"/>
     </row>
-    <row r="156" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>637</v>
       </c>
@@ -16269,7 +16053,7 @@
       <c r="W156" s="1"/>
       <c r="X156" s="1"/>
     </row>
-    <row r="157" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>637</v>
       </c>
@@ -16327,7 +16111,7 @@
       <c r="W157" s="1"/>
       <c r="X157" s="1"/>
     </row>
-    <row r="158" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>637</v>
       </c>
@@ -16385,7 +16169,7 @@
       <c r="W158" s="1"/>
       <c r="X158" s="1"/>
     </row>
-    <row r="159" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>637</v>
       </c>
@@ -16443,7 +16227,7 @@
       <c r="W159" s="1"/>
       <c r="X159" s="1"/>
     </row>
-    <row r="160" spans="1:24" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>637</v>
       </c>
@@ -16501,7 +16285,7 @@
       <c r="W160" s="1"/>
       <c r="X160" s="1"/>
     </row>
-    <row r="161" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>637</v>
       </c>
@@ -16559,7 +16343,7 @@
       <c r="W161" s="1"/>
       <c r="X161" s="1"/>
     </row>
-    <row r="162" spans="1:24" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>637</v>
       </c>
@@ -16617,7 +16401,7 @@
       <c r="W162" s="1"/>
       <c r="X162" s="1"/>
     </row>
-    <row r="163" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>637</v>
       </c>
@@ -16675,7 +16459,7 @@
       <c r="W163" s="1"/>
       <c r="X163" s="1"/>
     </row>
-    <row r="164" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>637</v>
       </c>
@@ -16733,7 +16517,7 @@
       <c r="W164" s="1"/>
       <c r="X164" s="1"/>
     </row>
-    <row r="165" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>637</v>
       </c>
@@ -16791,7 +16575,7 @@
       <c r="W165" s="1"/>
       <c r="X165" s="1"/>
     </row>
-    <row r="166" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>637</v>
       </c>
@@ -16849,7 +16633,7 @@
       <c r="W166" s="1"/>
       <c r="X166" s="1"/>
     </row>
-    <row r="167" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>637</v>
       </c>
@@ -16907,7 +16691,7 @@
       <c r="W167" s="1"/>
       <c r="X167" s="1"/>
     </row>
-    <row r="168" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>637</v>
       </c>
@@ -16965,7 +16749,7 @@
       <c r="W168" s="1"/>
       <c r="X168" s="1"/>
     </row>
-    <row r="169" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>637</v>
       </c>
@@ -17021,7 +16805,7 @@
       <c r="W169" s="1"/>
       <c r="X169" s="1"/>
     </row>
-    <row r="170" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>637</v>
       </c>
@@ -17077,7 +16861,7 @@
       <c r="W170" s="1"/>
       <c r="X170" s="1"/>
     </row>
-    <row r="171" spans="1:24" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>637</v>
       </c>
@@ -17135,7 +16919,7 @@
       <c r="W171" s="1"/>
       <c r="X171" s="1"/>
     </row>
-    <row r="172" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>637</v>
       </c>
@@ -17193,7 +16977,7 @@
       <c r="W172" s="1"/>
       <c r="X172" s="1"/>
     </row>
-    <row r="173" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>637</v>
       </c>
@@ -17251,7 +17035,7 @@
       <c r="W173" s="1"/>
       <c r="X173" s="1"/>
     </row>
-    <row r="174" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>637</v>
       </c>
@@ -17309,7 +17093,7 @@
       <c r="W174" s="1"/>
       <c r="X174" s="1"/>
     </row>
-    <row r="175" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>637</v>
       </c>
@@ -17367,7 +17151,7 @@
       <c r="W175" s="1"/>
       <c r="X175" s="1"/>
     </row>
-    <row r="176" spans="1:24" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>637</v>
       </c>
@@ -17425,7 +17209,7 @@
       <c r="W176" s="1"/>
       <c r="X176" s="1"/>
     </row>
-    <row r="177" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>637</v>
       </c>
@@ -17483,7 +17267,7 @@
       <c r="W177" s="1"/>
       <c r="X177" s="1"/>
     </row>
-    <row r="178" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>637</v>
       </c>
@@ -17541,7 +17325,7 @@
       <c r="W178" s="1"/>
       <c r="X178" s="1"/>
     </row>
-    <row r="179" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>637</v>
       </c>
@@ -17599,7 +17383,7 @@
       <c r="W179" s="1"/>
       <c r="X179" s="1"/>
     </row>
-    <row r="180" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>637</v>
       </c>
@@ -17657,7 +17441,7 @@
       <c r="W180" s="1"/>
       <c r="X180" s="1"/>
     </row>
-    <row r="181" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>637</v>
       </c>
@@ -17715,7 +17499,7 @@
       <c r="W181" s="1"/>
       <c r="X181" s="1"/>
     </row>
-    <row r="182" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>637</v>
       </c>
@@ -17773,7 +17557,7 @@
       <c r="W182" s="1"/>
       <c r="X182" s="1"/>
     </row>
-    <row r="183" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>637</v>
       </c>
@@ -17831,7 +17615,7 @@
       <c r="W183" s="1"/>
       <c r="X183" s="1"/>
     </row>
-    <row r="184" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>637</v>
       </c>
@@ -17889,7 +17673,7 @@
       <c r="W184" s="1"/>
       <c r="X184" s="1"/>
     </row>
-    <row r="185" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>637</v>
       </c>
@@ -17947,7 +17731,7 @@
       <c r="W185" s="1"/>
       <c r="X185" s="1"/>
     </row>
-    <row r="186" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>637</v>
       </c>
@@ -18005,7 +17789,7 @@
       <c r="W186" s="1"/>
       <c r="X186" s="1"/>
     </row>
-    <row r="187" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>637</v>
       </c>
@@ -18063,7 +17847,7 @@
       <c r="W187" s="1"/>
       <c r="X187" s="1"/>
     </row>
-    <row r="188" spans="1:24" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>637</v>
       </c>
@@ -18088,7 +17872,9 @@
       <c r="H188" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="I188" s="2"/>
+      <c r="I188" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J188" s="2" t="s">
         <v>1805</v>
       </c>
@@ -18131,7 +17917,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>637</v>
       </c>
@@ -18189,7 +17975,7 @@
       <c r="W189" s="1"/>
       <c r="X189" s="1"/>
     </row>
-    <row r="190" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>637</v>
       </c>
@@ -18247,7 +18033,7 @@
       <c r="W190" s="1"/>
       <c r="X190" s="1"/>
     </row>
-    <row r="191" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>637</v>
       </c>
@@ -18305,7 +18091,7 @@
       <c r="W191" s="1"/>
       <c r="X191" s="1"/>
     </row>
-    <row r="192" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>637</v>
       </c>
@@ -18363,7 +18149,7 @@
       <c r="W192" s="1"/>
       <c r="X192" s="1"/>
     </row>
-    <row r="193" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>637</v>
       </c>
@@ -18421,7 +18207,7 @@
       <c r="W193" s="1"/>
       <c r="X193" s="1"/>
     </row>
-    <row r="194" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>637</v>
       </c>
@@ -18479,7 +18265,7 @@
       <c r="W194" s="1"/>
       <c r="X194" s="1"/>
     </row>
-    <row r="195" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>637</v>
       </c>
@@ -18537,7 +18323,7 @@
       <c r="W195" s="1"/>
       <c r="X195" s="1"/>
     </row>
-    <row r="196" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>637</v>
       </c>
@@ -18595,7 +18381,7 @@
       <c r="W196" s="1"/>
       <c r="X196" s="1"/>
     </row>
-    <row r="197" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>637</v>
       </c>
@@ -18653,7 +18439,7 @@
       <c r="W197" s="1"/>
       <c r="X197" s="1"/>
     </row>
-    <row r="198" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>637</v>
       </c>
@@ -18711,7 +18497,7 @@
       <c r="W198" s="1"/>
       <c r="X198" s="1"/>
     </row>
-    <row r="199" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>637</v>
       </c>
@@ -18769,7 +18555,7 @@
       <c r="W199" s="1"/>
       <c r="X199" s="1"/>
     </row>
-    <row r="200" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>637</v>
       </c>
@@ -18827,7 +18613,7 @@
       <c r="W200" s="1"/>
       <c r="X200" s="1"/>
     </row>
-    <row r="201" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>637</v>
       </c>
@@ -18885,7 +18671,7 @@
       <c r="W201" s="1"/>
       <c r="X201" s="1"/>
     </row>
-    <row r="202" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>637</v>
       </c>
@@ -18943,7 +18729,7 @@
       <c r="W202" s="1"/>
       <c r="X202" s="1"/>
     </row>
-    <row r="203" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>637</v>
       </c>
@@ -19001,7 +18787,7 @@
       <c r="W203" s="1"/>
       <c r="X203" s="1"/>
     </row>
-    <row r="204" spans="1:24" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>637</v>
       </c>
@@ -19026,7 +18812,9 @@
       <c r="H204" s="2" t="s">
         <v>1432</v>
       </c>
-      <c r="I204" s="2"/>
+      <c r="I204" s="2" t="s">
+        <v>1860</v>
+      </c>
       <c r="J204" s="2" t="s">
         <v>1814</v>
       </c>
@@ -19069,7 +18857,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="205" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>637</v>
       </c>
@@ -19094,7 +18882,9 @@
       <c r="H205" s="2" t="s">
         <v>1437</v>
       </c>
-      <c r="I205" s="2"/>
+      <c r="I205" s="2" t="s">
+        <v>1861</v>
+      </c>
       <c r="J205" s="2" t="s">
         <v>1814</v>
       </c>
@@ -19133,9 +18923,11 @@
       <c r="W205" s="1" t="s">
         <v>1815</v>
       </c>
-      <c r="X205" s="1"/>
-    </row>
-    <row r="206" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X205" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="206" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>637</v>
       </c>
@@ -19193,7 +18985,7 @@
       <c r="W206" s="1"/>
       <c r="X206" s="1"/>
     </row>
-    <row r="207" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>637</v>
       </c>
@@ -19251,7 +19043,7 @@
       <c r="W207" s="1"/>
       <c r="X207" s="1"/>
     </row>
-    <row r="208" spans="1:24" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>637</v>
       </c>
@@ -19309,7 +19101,7 @@
       <c r="W208" s="1"/>
       <c r="X208" s="1"/>
     </row>
-    <row r="209" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>637</v>
       </c>
@@ -19367,7 +19159,7 @@
       <c r="W209" s="1"/>
       <c r="X209" s="1"/>
     </row>
-    <row r="210" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>637</v>
       </c>
@@ -19425,7 +19217,7 @@
       <c r="W210" s="1"/>
       <c r="X210" s="1"/>
     </row>
-    <row r="211" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>637</v>
       </c>
@@ -19483,7 +19275,7 @@
       <c r="W211" s="1"/>
       <c r="X211" s="1"/>
     </row>
-    <row r="212" spans="1:24" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>637</v>
       </c>
@@ -19541,7 +19333,7 @@
       <c r="W212" s="1"/>
       <c r="X212" s="1"/>
     </row>
-    <row r="213" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>637</v>
       </c>
@@ -19599,7 +19391,7 @@
       <c r="W213" s="1"/>
       <c r="X213" s="1"/>
     </row>
-    <row r="214" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>637</v>
       </c>
@@ -19657,7 +19449,7 @@
       <c r="W214" s="1"/>
       <c r="X214" s="1"/>
     </row>
-    <row r="215" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>637</v>
       </c>
@@ -19715,7 +19507,7 @@
       <c r="W215" s="1"/>
       <c r="X215" s="1"/>
     </row>
-    <row r="216" spans="1:24" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>637</v>
       </c>
@@ -19773,7 +19565,7 @@
       <c r="W216" s="1"/>
       <c r="X216" s="1"/>
     </row>
-    <row r="217" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>637</v>
       </c>
@@ -19831,7 +19623,7 @@
       <c r="W217" s="1"/>
       <c r="X217" s="1"/>
     </row>
-    <row r="218" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>637</v>
       </c>
@@ -19889,7 +19681,7 @@
       <c r="W218" s="1"/>
       <c r="X218" s="1"/>
     </row>
-    <row r="219" spans="1:24" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>637</v>
       </c>
@@ -19947,7 +19739,7 @@
       <c r="W219" s="1"/>
       <c r="X219" s="1"/>
     </row>
-    <row r="220" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>637</v>
       </c>
@@ -20005,7 +19797,7 @@
       <c r="W220" s="1"/>
       <c r="X220" s="1"/>
     </row>
-    <row r="221" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>637</v>
       </c>
@@ -20063,7 +19855,7 @@
       <c r="W221" s="1"/>
       <c r="X221" s="1"/>
     </row>
-    <row r="222" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>637</v>
       </c>
@@ -20121,7 +19913,7 @@
       <c r="W222" s="1"/>
       <c r="X222" s="1"/>
     </row>
-    <row r="223" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>637</v>
       </c>
@@ -20179,7 +19971,7 @@
       <c r="W223" s="1"/>
       <c r="X223" s="1"/>
     </row>
-    <row r="224" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>637</v>
       </c>
@@ -20237,7 +20029,7 @@
       <c r="W224" s="1"/>
       <c r="X224" s="1"/>
     </row>
-    <row r="225" spans="1:24" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>637</v>
       </c>
@@ -20295,7 +20087,7 @@
       <c r="W225" s="1"/>
       <c r="X225" s="1"/>
     </row>
-    <row r="226" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>637</v>
       </c>
@@ -20353,7 +20145,7 @@
       <c r="W226" s="1"/>
       <c r="X226" s="1"/>
     </row>
-    <row r="227" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>637</v>
       </c>
@@ -20411,7 +20203,7 @@
       <c r="W227" s="1"/>
       <c r="X227" s="1"/>
     </row>
-    <row r="228" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>637</v>
       </c>
@@ -20469,7 +20261,7 @@
       <c r="W228" s="1"/>
       <c r="X228" s="1"/>
     </row>
-    <row r="229" spans="1:24" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>637</v>
       </c>
@@ -20494,12 +20286,14 @@
       <c r="H229" s="2" t="s">
         <v>1614</v>
       </c>
-      <c r="I229" s="2"/>
+      <c r="I229" s="2" t="s">
+        <v>1859</v>
+      </c>
       <c r="J229" s="2" t="s">
         <v>1810</v>
       </c>
       <c r="K229" s="2" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="L229" s="2" t="s">
         <v>1817</v>
@@ -20537,7 +20331,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="230" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>637</v>
       </c>
@@ -20595,7 +20389,7 @@
       <c r="W230" s="1"/>
       <c r="X230" s="1"/>
     </row>
-    <row r="231" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>637</v>
       </c>
@@ -20653,7 +20447,7 @@
       <c r="W231" s="1"/>
       <c r="X231" s="1"/>
     </row>
-    <row r="232" spans="1:24" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>637</v>
       </c>
@@ -20711,7 +20505,7 @@
       <c r="W232" s="1"/>
       <c r="X232" s="1"/>
     </row>
-    <row r="233" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>637</v>
       </c>
@@ -20769,7 +20563,7 @@
       <c r="W233" s="1"/>
       <c r="X233" s="1"/>
     </row>
-    <row r="234" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>637</v>
       </c>
@@ -20827,7 +20621,7 @@
       <c r="W234" s="1"/>
       <c r="X234" s="1"/>
     </row>
-    <row r="235" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>637</v>
       </c>
@@ -20885,7 +20679,7 @@
       <c r="W235" s="1"/>
       <c r="X235" s="1"/>
     </row>
-    <row r="236" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>637</v>
       </c>
@@ -20943,7 +20737,7 @@
       <c r="W236" s="1"/>
       <c r="X236" s="1"/>
     </row>
-    <row r="237" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>637</v>
       </c>
@@ -21001,7 +20795,7 @@
       <c r="W237" s="1"/>
       <c r="X237" s="1"/>
     </row>
-    <row r="238" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>637</v>
       </c>
@@ -21059,7 +20853,7 @@
       <c r="W238" s="1"/>
       <c r="X238" s="1"/>
     </row>
-    <row r="239" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>637</v>
       </c>
@@ -21117,7 +20911,7 @@
       <c r="W239" s="1"/>
       <c r="X239" s="1"/>
     </row>
-    <row r="240" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>637</v>
       </c>
@@ -21175,7 +20969,7 @@
       <c r="W240" s="1"/>
       <c r="X240" s="1"/>
     </row>
-    <row r="241" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>637</v>
       </c>
@@ -21233,7 +21027,7 @@
       <c r="W241" s="1"/>
       <c r="X241" s="1"/>
     </row>
-    <row r="242" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>637</v>
       </c>
@@ -21291,7 +21085,7 @@
       <c r="W242" s="1"/>
       <c r="X242" s="1"/>
     </row>
-    <row r="243" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>637</v>
       </c>
@@ -21349,7 +21143,7 @@
       <c r="W243" s="1"/>
       <c r="X243" s="1"/>
     </row>
-    <row r="244" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>637</v>
       </c>
@@ -21407,7 +21201,7 @@
       <c r="W244" s="1"/>
       <c r="X244" s="1"/>
     </row>
-    <row r="245" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>637</v>
       </c>
@@ -21465,7 +21259,7 @@
       <c r="W245" s="1"/>
       <c r="X245" s="1"/>
     </row>
-    <row r="246" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>637</v>
       </c>
@@ -21523,7 +21317,7 @@
       <c r="W246" s="1"/>
       <c r="X246" s="1"/>
     </row>
-    <row r="247" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>637</v>
       </c>
@@ -21581,7 +21375,7 @@
       <c r="W247" s="1"/>
       <c r="X247" s="1"/>
     </row>
-    <row r="248" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>637</v>
       </c>
@@ -21639,7 +21433,7 @@
       <c r="W248" s="1"/>
       <c r="X248" s="1"/>
     </row>
-    <row r="249" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>637</v>
       </c>
@@ -21697,7 +21491,7 @@
       <c r="W249" s="1"/>
       <c r="X249" s="1"/>
     </row>
-    <row r="250" spans="1:24" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>637</v>
       </c>
@@ -21755,7 +21549,7 @@
       <c r="W250" s="1"/>
       <c r="X250" s="1"/>
     </row>
-    <row r="251" spans="1:24" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>637</v>
       </c>
@@ -21813,7 +21607,7 @@
       <c r="W251" s="1"/>
       <c r="X251" s="1"/>
     </row>
-    <row r="252" spans="1:24" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>637</v>
       </c>
@@ -21871,7 +21665,7 @@
       <c r="W252" s="1"/>
       <c r="X252" s="1"/>
     </row>
-    <row r="253" spans="1:24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>637</v>
       </c>
@@ -21929,7 +21723,7 @@
       <c r="W253" s="1"/>
       <c r="X253" s="1"/>
     </row>
-    <row r="254" spans="1:24" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>1786</v>
       </c>
@@ -21989,18 +21783,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:X254" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="10">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="23">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A84:X127">
-      <sortCondition ref="G1:G254"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A102:X149">
+      <sortCondition ref="B1:B254"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
adds drinventor corpus and first papers
</commit_message>
<xml_diff>
--- a/data/ReferenceErrorDetection_data_annotated.xlsx
+++ b/data/ReferenceErrorDetection_data_annotated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Masterarbeit\citation-verification\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b78b8e360351019/_Dokumente/Studium/Master/Masterarbeit/_citation-verification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C74259B-E541-49C6-92FD-3E8C145AE8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{3C74259B-E541-49C6-92FD-3E8C145AE8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BCBB0D8-C402-4CAB-BDCC-E9150A86FFAF}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1710" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5953,6 +5953,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6240,9 +6244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:X254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A188" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
@@ -6250,6 +6255,7 @@
   <cols>
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="54.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="9" width="56.85546875" style="5" customWidth="1"/>
     <col min="10" max="12" width="25.42578125" style="5" customWidth="1"/>
@@ -6339,7 +6345,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -6399,7 +6405,7 @@
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
     </row>
-    <row r="3" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -6459,7 +6465,7 @@
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
     </row>
-    <row r="4" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -6519,7 +6525,7 @@
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
     </row>
-    <row r="5" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -6579,7 +6585,7 @@
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
     </row>
-    <row r="6" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -6639,7 +6645,7 @@
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
     </row>
-    <row r="7" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -6699,7 +6705,7 @@
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
     </row>
-    <row r="8" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -6759,7 +6765,7 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
     </row>
-    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -6819,7 +6825,7 @@
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
     </row>
-    <row r="10" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -6879,7 +6885,7 @@
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
     </row>
-    <row r="11" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -6939,7 +6945,7 @@
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
     </row>
-    <row r="12" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -6999,7 +7005,7 @@
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
     </row>
-    <row r="13" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -7059,7 +7065,7 @@
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
     </row>
-    <row r="14" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -7119,7 +7125,7 @@
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
     </row>
-    <row r="15" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -7179,7 +7185,7 @@
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
     </row>
-    <row r="16" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -7239,7 +7245,7 @@
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
     </row>
-    <row r="17" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -7299,7 +7305,7 @@
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
     </row>
-    <row r="18" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -7359,7 +7365,7 @@
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
     </row>
-    <row r="19" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -7419,7 +7425,7 @@
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
     </row>
-    <row r="20" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -7479,7 +7485,7 @@
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
     </row>
-    <row r="21" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -7539,7 +7545,7 @@
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
     </row>
-    <row r="22" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -7599,7 +7605,7 @@
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
     </row>
-    <row r="23" spans="1:24" ht="120" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -7659,7 +7665,7 @@
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
     </row>
-    <row r="24" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -7719,7 +7725,7 @@
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
     </row>
-    <row r="25" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -7851,7 +7857,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
@@ -7911,7 +7917,7 @@
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
     </row>
-    <row r="28" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
@@ -8253,7 +8259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
@@ -8313,7 +8319,7 @@
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
     </row>
-    <row r="34" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -8373,7 +8379,7 @@
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
     </row>
-    <row r="35" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
@@ -8433,7 +8439,7 @@
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
     </row>
-    <row r="36" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>17</v>
       </c>
@@ -8493,7 +8499,7 @@
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
     </row>
-    <row r="37" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -8553,7 +8559,7 @@
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
     </row>
-    <row r="38" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>17</v>
       </c>
@@ -8613,7 +8619,7 @@
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
     </row>
-    <row r="39" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>17</v>
       </c>
@@ -8673,7 +8679,7 @@
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
     </row>
-    <row r="40" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -8733,7 +8739,7 @@
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
     </row>
-    <row r="41" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -8793,7 +8799,7 @@
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
     </row>
-    <row r="42" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
@@ -8853,7 +8859,7 @@
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
     </row>
-    <row r="43" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
@@ -8913,7 +8919,7 @@
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
     </row>
-    <row r="44" spans="1:24" ht="105" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>17</v>
       </c>
@@ -8973,7 +8979,7 @@
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
     </row>
-    <row r="45" spans="1:24" ht="105" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>17</v>
       </c>
@@ -9033,7 +9039,7 @@
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
     </row>
-    <row r="46" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
@@ -9093,7 +9099,7 @@
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
     </row>
-    <row r="47" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>17</v>
       </c>
@@ -9153,7 +9159,7 @@
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
     </row>
-    <row r="48" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>17</v>
       </c>
@@ -9225,7 +9231,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>17</v>
       </c>
@@ -9297,7 +9303,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>17</v>
       </c>
@@ -9357,7 +9363,7 @@
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
     </row>
-    <row r="51" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>17</v>
       </c>
@@ -9417,7 +9423,7 @@
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
     </row>
-    <row r="52" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>17</v>
       </c>
@@ -9477,7 +9483,7 @@
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
     </row>
-    <row r="53" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>17</v>
       </c>
@@ -9537,7 +9543,7 @@
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
     </row>
-    <row r="54" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>17</v>
       </c>
@@ -9609,7 +9615,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="315" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>17</v>
       </c>
@@ -9679,7 +9685,7 @@
         <v>1835</v>
       </c>
     </row>
-    <row r="56" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>17</v>
       </c>
@@ -9739,7 +9745,7 @@
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
     </row>
-    <row r="57" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>17</v>
       </c>
@@ -9799,7 +9805,7 @@
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
     </row>
-    <row r="58" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>17</v>
       </c>
@@ -9859,7 +9865,7 @@
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
     </row>
-    <row r="59" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>17</v>
       </c>
@@ -9919,7 +9925,7 @@
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
     </row>
-    <row r="60" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>17</v>
       </c>
@@ -9979,7 +9985,7 @@
       <c r="W60" s="1"/>
       <c r="X60" s="1"/>
     </row>
-    <row r="61" spans="1:24" ht="105" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>17</v>
       </c>
@@ -10039,7 +10045,7 @@
       <c r="W61" s="1"/>
       <c r="X61" s="1"/>
     </row>
-    <row r="62" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>17</v>
       </c>
@@ -10099,7 +10105,7 @@
       <c r="W62" s="1"/>
       <c r="X62" s="1"/>
     </row>
-    <row r="63" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>17</v>
       </c>
@@ -10159,7 +10165,7 @@
       <c r="W63" s="1"/>
       <c r="X63" s="1"/>
     </row>
-    <row r="64" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>17</v>
       </c>
@@ -10219,7 +10225,7 @@
       <c r="W64" s="1"/>
       <c r="X64" s="1"/>
     </row>
-    <row r="65" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>17</v>
       </c>
@@ -10279,7 +10285,7 @@
       <c r="W65" s="1"/>
       <c r="X65" s="1"/>
     </row>
-    <row r="66" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>17</v>
       </c>
@@ -10339,7 +10345,7 @@
       <c r="W66" s="1"/>
       <c r="X66" s="1"/>
     </row>
-    <row r="67" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>17</v>
       </c>
@@ -10399,7 +10405,7 @@
       <c r="W67" s="1"/>
       <c r="X67" s="1"/>
     </row>
-    <row r="68" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>17</v>
       </c>
@@ -10891,7 +10897,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>17</v>
       </c>
@@ -10951,7 +10957,7 @@
       <c r="W75" s="1"/>
       <c r="X75" s="1"/>
     </row>
-    <row r="76" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>17</v>
       </c>
@@ -11011,7 +11017,7 @@
       <c r="W76" s="1"/>
       <c r="X76" s="1"/>
     </row>
-    <row r="77" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>17</v>
       </c>
@@ -11069,7 +11075,7 @@
       <c r="W77" s="1"/>
       <c r="X77" s="1"/>
     </row>
-    <row r="78" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>17</v>
       </c>
@@ -11129,7 +11135,7 @@
       <c r="W78" s="1"/>
       <c r="X78" s="1"/>
     </row>
-    <row r="79" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>17</v>
       </c>
@@ -11189,7 +11195,7 @@
       <c r="W79" s="1"/>
       <c r="X79" s="1"/>
     </row>
-    <row r="80" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -11249,7 +11255,7 @@
       <c r="W80" s="1"/>
       <c r="X80" s="1"/>
     </row>
-    <row r="81" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>17</v>
       </c>
@@ -11309,7 +11315,7 @@
       <c r="W81" s="1"/>
       <c r="X81" s="1"/>
     </row>
-    <row r="82" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>17</v>
       </c>
@@ -11369,7 +11375,7 @@
       <c r="W82" s="1"/>
       <c r="X82" s="1"/>
     </row>
-    <row r="83" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>541</v>
       </c>
@@ -11431,7 +11437,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="84" spans="1:24" ht="300" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>637</v>
       </c>
@@ -11501,7 +11507,7 @@
         <v>1835</v>
       </c>
     </row>
-    <row r="85" spans="1:24" ht="300" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>637</v>
       </c>
@@ -11575,7 +11581,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>637</v>
       </c>
@@ -11645,7 +11651,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="87" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>637</v>
       </c>
@@ -11717,7 +11723,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>637</v>
       </c>
@@ -11789,7 +11795,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>541</v>
       </c>
@@ -11861,7 +11867,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>541</v>
       </c>
@@ -11933,7 +11939,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>584</v>
       </c>
@@ -12005,7 +12011,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>584</v>
       </c>
@@ -12077,7 +12083,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>601</v>
       </c>
@@ -12149,7 +12155,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>611</v>
       </c>
@@ -12221,7 +12227,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>621</v>
       </c>
@@ -12279,7 +12285,7 @@
       <c r="W95" s="1"/>
       <c r="X95" s="1"/>
     </row>
-    <row r="96" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>621</v>
       </c>
@@ -12337,7 +12343,7 @@
       <c r="W96" s="1"/>
       <c r="X96" s="1"/>
     </row>
-    <row r="97" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>621</v>
       </c>
@@ -12395,7 +12401,7 @@
       <c r="W97" s="1"/>
       <c r="X97" s="1"/>
     </row>
-    <row r="98" spans="1:24" ht="405" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:24" ht="405" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>637</v>
       </c>
@@ -12467,7 +12473,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="99" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>541</v>
       </c>
@@ -12539,7 +12545,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>637</v>
       </c>
@@ -12597,7 +12603,7 @@
       <c r="W100" s="1"/>
       <c r="X100" s="1"/>
     </row>
-    <row r="101" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>637</v>
       </c>
@@ -12657,7 +12663,7 @@
       <c r="W101" s="1"/>
       <c r="X101" s="1"/>
     </row>
-    <row r="102" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>541</v>
       </c>
@@ -12729,7 +12735,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="103" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>637</v>
       </c>
@@ -12785,7 +12791,7 @@
       <c r="W103" s="1"/>
       <c r="X103" s="1"/>
     </row>
-    <row r="104" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>637</v>
       </c>
@@ -12843,7 +12849,7 @@
       <c r="W104" s="1"/>
       <c r="X104" s="1"/>
     </row>
-    <row r="105" spans="1:24" ht="225" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:24" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>637</v>
       </c>
@@ -12913,7 +12919,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="106" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>541</v>
       </c>
@@ -12985,7 +12991,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="107" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>637</v>
       </c>
@@ -13043,7 +13049,7 @@
       <c r="W107" s="1"/>
       <c r="X107" s="1"/>
     </row>
-    <row r="108" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>637</v>
       </c>
@@ -13115,7 +13121,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>637</v>
       </c>
@@ -13175,7 +13181,7 @@
       <c r="W109" s="1"/>
       <c r="X109" s="1"/>
     </row>
-    <row r="110" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>637</v>
       </c>
@@ -13233,7 +13239,7 @@
       <c r="W110" s="1"/>
       <c r="X110" s="1"/>
     </row>
-    <row r="111" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>541</v>
       </c>
@@ -13305,7 +13311,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>637</v>
       </c>
@@ -13363,7 +13369,7 @@
       <c r="W112" s="1"/>
       <c r="X112" s="1"/>
     </row>
-    <row r="113" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>637</v>
       </c>
@@ -13421,7 +13427,7 @@
       <c r="W113" s="1"/>
       <c r="X113" s="1"/>
     </row>
-    <row r="114" spans="1:24" ht="210" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>637</v>
       </c>
@@ -13493,7 +13499,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="115" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>637</v>
       </c>
@@ -13551,7 +13557,7 @@
       <c r="W115" s="1"/>
       <c r="X115" s="1"/>
     </row>
-    <row r="116" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>637</v>
       </c>
@@ -13611,7 +13617,7 @@
       <c r="W116" s="1"/>
       <c r="X116" s="1"/>
     </row>
-    <row r="117" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>637</v>
       </c>
@@ -13669,7 +13675,7 @@
       <c r="W117" s="1"/>
       <c r="X117" s="1"/>
     </row>
-    <row r="118" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>637</v>
       </c>
@@ -13729,7 +13735,7 @@
       <c r="W118" s="1"/>
       <c r="X118" s="1"/>
     </row>
-    <row r="119" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>637</v>
       </c>
@@ -13787,7 +13793,7 @@
       <c r="W119" s="1"/>
       <c r="X119" s="1"/>
     </row>
-    <row r="120" spans="1:24" ht="105" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>637</v>
       </c>
@@ -13845,7 +13851,7 @@
       <c r="W120" s="1"/>
       <c r="X120" s="1"/>
     </row>
-    <row r="121" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>637</v>
       </c>
@@ -13905,7 +13911,7 @@
       <c r="W121" s="1"/>
       <c r="X121" s="1"/>
     </row>
-    <row r="122" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>637</v>
       </c>
@@ -13963,7 +13969,7 @@
       <c r="W122" s="1"/>
       <c r="X122" s="1"/>
     </row>
-    <row r="123" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>637</v>
       </c>
@@ -14021,7 +14027,7 @@
       <c r="W123" s="1"/>
       <c r="X123" s="1"/>
     </row>
-    <row r="124" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>637</v>
       </c>
@@ -14081,7 +14087,7 @@
       <c r="W124" s="1"/>
       <c r="X124" s="1"/>
     </row>
-    <row r="125" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>637</v>
       </c>
@@ -14149,7 +14155,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="126" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>637</v>
       </c>
@@ -14209,7 +14215,7 @@
       <c r="W126" s="1"/>
       <c r="X126" s="1"/>
     </row>
-    <row r="127" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>637</v>
       </c>
@@ -14281,7 +14287,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="128" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>637</v>
       </c>
@@ -14341,7 +14347,7 @@
       <c r="W128" s="1"/>
       <c r="X128" s="1"/>
     </row>
-    <row r="129" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>637</v>
       </c>
@@ -14411,7 +14417,7 @@
         <v>1835</v>
       </c>
     </row>
-    <row r="130" spans="1:24" ht="135" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>637</v>
       </c>
@@ -14481,7 +14487,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="131" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>637</v>
       </c>
@@ -14541,7 +14547,7 @@
       <c r="W131" s="1"/>
       <c r="X131" s="1"/>
     </row>
-    <row r="132" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>637</v>
       </c>
@@ -14613,7 +14619,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="133" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>637</v>
       </c>
@@ -14673,7 +14679,7 @@
       <c r="W133" s="1"/>
       <c r="X133" s="1"/>
     </row>
-    <row r="134" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>637</v>
       </c>
@@ -14733,7 +14739,7 @@
       <c r="W134" s="1"/>
       <c r="X134" s="1"/>
     </row>
-    <row r="135" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>637</v>
       </c>
@@ -14805,7 +14811,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="136" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>637</v>
       </c>
@@ -14863,7 +14869,7 @@
       <c r="W136" s="1"/>
       <c r="X136" s="1"/>
     </row>
-    <row r="137" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>637</v>
       </c>
@@ -14921,7 +14927,7 @@
       <c r="W137" s="1"/>
       <c r="X137" s="1"/>
     </row>
-    <row r="138" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>637</v>
       </c>
@@ -14979,7 +14985,7 @@
       <c r="W138" s="1"/>
       <c r="X138" s="1"/>
     </row>
-    <row r="139" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>637</v>
       </c>
@@ -15037,7 +15043,7 @@
       <c r="W139" s="1"/>
       <c r="X139" s="1"/>
     </row>
-    <row r="140" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>637</v>
       </c>
@@ -15095,7 +15101,7 @@
       <c r="W140" s="1"/>
       <c r="X140" s="1"/>
     </row>
-    <row r="141" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>637</v>
       </c>
@@ -15155,7 +15161,7 @@
       <c r="W141" s="1"/>
       <c r="X141" s="1"/>
     </row>
-    <row r="142" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>637</v>
       </c>
@@ -15213,7 +15219,7 @@
       <c r="W142" s="1"/>
       <c r="X142" s="1"/>
     </row>
-    <row r="143" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>637</v>
       </c>
@@ -15273,7 +15279,7 @@
       <c r="W143" s="1"/>
       <c r="X143" s="1"/>
     </row>
-    <row r="144" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>637</v>
       </c>
@@ -15333,7 +15339,7 @@
       <c r="W144" s="1"/>
       <c r="X144" s="1"/>
     </row>
-    <row r="145" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>637</v>
       </c>
@@ -15391,7 +15397,7 @@
       <c r="W145" s="1"/>
       <c r="X145" s="1"/>
     </row>
-    <row r="146" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>637</v>
       </c>
@@ -15451,7 +15457,7 @@
       <c r="W146" s="1"/>
       <c r="X146" s="1"/>
     </row>
-    <row r="147" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>637</v>
       </c>
@@ -15509,7 +15515,7 @@
       <c r="W147" s="1"/>
       <c r="X147" s="1"/>
     </row>
-    <row r="148" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>637</v>
       </c>
@@ -15569,7 +15575,7 @@
       <c r="W148" s="1"/>
       <c r="X148" s="1"/>
     </row>
-    <row r="149" spans="1:24" ht="225" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:24" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>637</v>
       </c>
@@ -15639,7 +15645,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="150" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>637</v>
       </c>
@@ -15699,7 +15705,7 @@
       <c r="W150" s="1"/>
       <c r="X150" s="1"/>
     </row>
-    <row r="151" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>637</v>
       </c>
@@ -15759,7 +15765,7 @@
       <c r="W151" s="1"/>
       <c r="X151" s="1"/>
     </row>
-    <row r="152" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>637</v>
       </c>
@@ -15819,7 +15825,7 @@
       <c r="W152" s="1"/>
       <c r="X152" s="1"/>
     </row>
-    <row r="153" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>637</v>
       </c>
@@ -15877,7 +15883,7 @@
       <c r="W153" s="1"/>
       <c r="X153" s="1"/>
     </row>
-    <row r="154" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>637</v>
       </c>
@@ -15937,7 +15943,7 @@
       <c r="W154" s="1"/>
       <c r="X154" s="1"/>
     </row>
-    <row r="155" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>637</v>
       </c>
@@ -15995,7 +16001,7 @@
       <c r="W155" s="1"/>
       <c r="X155" s="1"/>
     </row>
-    <row r="156" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>637</v>
       </c>
@@ -16053,7 +16059,7 @@
       <c r="W156" s="1"/>
       <c r="X156" s="1"/>
     </row>
-    <row r="157" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>637</v>
       </c>
@@ -16111,7 +16117,7 @@
       <c r="W157" s="1"/>
       <c r="X157" s="1"/>
     </row>
-    <row r="158" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>637</v>
       </c>
@@ -16169,7 +16175,7 @@
       <c r="W158" s="1"/>
       <c r="X158" s="1"/>
     </row>
-    <row r="159" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>637</v>
       </c>
@@ -16227,7 +16233,7 @@
       <c r="W159" s="1"/>
       <c r="X159" s="1"/>
     </row>
-    <row r="160" spans="1:24" ht="105" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:24" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>637</v>
       </c>
@@ -16285,7 +16291,7 @@
       <c r="W160" s="1"/>
       <c r="X160" s="1"/>
     </row>
-    <row r="161" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>637</v>
       </c>
@@ -16343,7 +16349,7 @@
       <c r="W161" s="1"/>
       <c r="X161" s="1"/>
     </row>
-    <row r="162" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>637</v>
       </c>
@@ -16401,7 +16407,7 @@
       <c r="W162" s="1"/>
       <c r="X162" s="1"/>
     </row>
-    <row r="163" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>637</v>
       </c>
@@ -16459,7 +16465,7 @@
       <c r="W163" s="1"/>
       <c r="X163" s="1"/>
     </row>
-    <row r="164" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>637</v>
       </c>
@@ -16517,7 +16523,7 @@
       <c r="W164" s="1"/>
       <c r="X164" s="1"/>
     </row>
-    <row r="165" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>637</v>
       </c>
@@ -16575,7 +16581,7 @@
       <c r="W165" s="1"/>
       <c r="X165" s="1"/>
     </row>
-    <row r="166" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>637</v>
       </c>
@@ -16633,7 +16639,7 @@
       <c r="W166" s="1"/>
       <c r="X166" s="1"/>
     </row>
-    <row r="167" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>637</v>
       </c>
@@ -16691,7 +16697,7 @@
       <c r="W167" s="1"/>
       <c r="X167" s="1"/>
     </row>
-    <row r="168" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>637</v>
       </c>
@@ -16749,7 +16755,7 @@
       <c r="W168" s="1"/>
       <c r="X168" s="1"/>
     </row>
-    <row r="169" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>637</v>
       </c>
@@ -16805,7 +16811,7 @@
       <c r="W169" s="1"/>
       <c r="X169" s="1"/>
     </row>
-    <row r="170" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>637</v>
       </c>
@@ -16861,7 +16867,7 @@
       <c r="W170" s="1"/>
       <c r="X170" s="1"/>
     </row>
-    <row r="171" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>637</v>
       </c>
@@ -16919,7 +16925,7 @@
       <c r="W171" s="1"/>
       <c r="X171" s="1"/>
     </row>
-    <row r="172" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>637</v>
       </c>
@@ -16977,7 +16983,7 @@
       <c r="W172" s="1"/>
       <c r="X172" s="1"/>
     </row>
-    <row r="173" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>637</v>
       </c>
@@ -17035,7 +17041,7 @@
       <c r="W173" s="1"/>
       <c r="X173" s="1"/>
     </row>
-    <row r="174" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>637</v>
       </c>
@@ -17093,7 +17099,7 @@
       <c r="W174" s="1"/>
       <c r="X174" s="1"/>
     </row>
-    <row r="175" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>637</v>
       </c>
@@ -17151,7 +17157,7 @@
       <c r="W175" s="1"/>
       <c r="X175" s="1"/>
     </row>
-    <row r="176" spans="1:24" ht="135" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:24" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>637</v>
       </c>
@@ -17209,7 +17215,7 @@
       <c r="W176" s="1"/>
       <c r="X176" s="1"/>
     </row>
-    <row r="177" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>637</v>
       </c>
@@ -17267,7 +17273,7 @@
       <c r="W177" s="1"/>
       <c r="X177" s="1"/>
     </row>
-    <row r="178" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>637</v>
       </c>
@@ -17325,7 +17331,7 @@
       <c r="W178" s="1"/>
       <c r="X178" s="1"/>
     </row>
-    <row r="179" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>637</v>
       </c>
@@ -17383,7 +17389,7 @@
       <c r="W179" s="1"/>
       <c r="X179" s="1"/>
     </row>
-    <row r="180" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>637</v>
       </c>
@@ -17441,7 +17447,7 @@
       <c r="W180" s="1"/>
       <c r="X180" s="1"/>
     </row>
-    <row r="181" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>637</v>
       </c>
@@ -17499,7 +17505,7 @@
       <c r="W181" s="1"/>
       <c r="X181" s="1"/>
     </row>
-    <row r="182" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>637</v>
       </c>
@@ -17557,7 +17563,7 @@
       <c r="W182" s="1"/>
       <c r="X182" s="1"/>
     </row>
-    <row r="183" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>637</v>
       </c>
@@ -17615,7 +17621,7 @@
       <c r="W183" s="1"/>
       <c r="X183" s="1"/>
     </row>
-    <row r="184" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>637</v>
       </c>
@@ -17673,7 +17679,7 @@
       <c r="W184" s="1"/>
       <c r="X184" s="1"/>
     </row>
-    <row r="185" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>637</v>
       </c>
@@ -17731,7 +17737,7 @@
       <c r="W185" s="1"/>
       <c r="X185" s="1"/>
     </row>
-    <row r="186" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>637</v>
       </c>
@@ -17789,7 +17795,7 @@
       <c r="W186" s="1"/>
       <c r="X186" s="1"/>
     </row>
-    <row r="187" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>637</v>
       </c>
@@ -17917,7 +17923,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>637</v>
       </c>
@@ -17975,7 +17981,7 @@
       <c r="W189" s="1"/>
       <c r="X189" s="1"/>
     </row>
-    <row r="190" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>637</v>
       </c>
@@ -18033,7 +18039,7 @@
       <c r="W190" s="1"/>
       <c r="X190" s="1"/>
     </row>
-    <row r="191" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>637</v>
       </c>
@@ -18091,7 +18097,7 @@
       <c r="W191" s="1"/>
       <c r="X191" s="1"/>
     </row>
-    <row r="192" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>637</v>
       </c>
@@ -18149,7 +18155,7 @@
       <c r="W192" s="1"/>
       <c r="X192" s="1"/>
     </row>
-    <row r="193" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>637</v>
       </c>
@@ -18207,7 +18213,7 @@
       <c r="W193" s="1"/>
       <c r="X193" s="1"/>
     </row>
-    <row r="194" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>637</v>
       </c>
@@ -18265,7 +18271,7 @@
       <c r="W194" s="1"/>
       <c r="X194" s="1"/>
     </row>
-    <row r="195" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>637</v>
       </c>
@@ -18323,7 +18329,7 @@
       <c r="W195" s="1"/>
       <c r="X195" s="1"/>
     </row>
-    <row r="196" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>637</v>
       </c>
@@ -18381,7 +18387,7 @@
       <c r="W196" s="1"/>
       <c r="X196" s="1"/>
     </row>
-    <row r="197" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>637</v>
       </c>
@@ -18439,7 +18445,7 @@
       <c r="W197" s="1"/>
       <c r="X197" s="1"/>
     </row>
-    <row r="198" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>637</v>
       </c>
@@ -18497,7 +18503,7 @@
       <c r="W198" s="1"/>
       <c r="X198" s="1"/>
     </row>
-    <row r="199" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>637</v>
       </c>
@@ -18555,7 +18561,7 @@
       <c r="W199" s="1"/>
       <c r="X199" s="1"/>
     </row>
-    <row r="200" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>637</v>
       </c>
@@ -18613,7 +18619,7 @@
       <c r="W200" s="1"/>
       <c r="X200" s="1"/>
     </row>
-    <row r="201" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>637</v>
       </c>
@@ -18671,7 +18677,7 @@
       <c r="W201" s="1"/>
       <c r="X201" s="1"/>
     </row>
-    <row r="202" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>637</v>
       </c>
@@ -18729,7 +18735,7 @@
       <c r="W202" s="1"/>
       <c r="X202" s="1"/>
     </row>
-    <row r="203" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>637</v>
       </c>
@@ -18927,7 +18933,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="206" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>637</v>
       </c>
@@ -18985,7 +18991,7 @@
       <c r="W206" s="1"/>
       <c r="X206" s="1"/>
     </row>
-    <row r="207" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>637</v>
       </c>
@@ -19043,7 +19049,7 @@
       <c r="W207" s="1"/>
       <c r="X207" s="1"/>
     </row>
-    <row r="208" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>637</v>
       </c>
@@ -19101,7 +19107,7 @@
       <c r="W208" s="1"/>
       <c r="X208" s="1"/>
     </row>
-    <row r="209" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>637</v>
       </c>
@@ -19159,7 +19165,7 @@
       <c r="W209" s="1"/>
       <c r="X209" s="1"/>
     </row>
-    <row r="210" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>637</v>
       </c>
@@ -19217,7 +19223,7 @@
       <c r="W210" s="1"/>
       <c r="X210" s="1"/>
     </row>
-    <row r="211" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>637</v>
       </c>
@@ -19275,7 +19281,7 @@
       <c r="W211" s="1"/>
       <c r="X211" s="1"/>
     </row>
-    <row r="212" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>637</v>
       </c>
@@ -19333,7 +19339,7 @@
       <c r="W212" s="1"/>
       <c r="X212" s="1"/>
     </row>
-    <row r="213" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>637</v>
       </c>
@@ -19391,7 +19397,7 @@
       <c r="W213" s="1"/>
       <c r="X213" s="1"/>
     </row>
-    <row r="214" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>637</v>
       </c>
@@ -19449,7 +19455,7 @@
       <c r="W214" s="1"/>
       <c r="X214" s="1"/>
     </row>
-    <row r="215" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>637</v>
       </c>
@@ -19507,7 +19513,7 @@
       <c r="W215" s="1"/>
       <c r="X215" s="1"/>
     </row>
-    <row r="216" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>637</v>
       </c>
@@ -19565,7 +19571,7 @@
       <c r="W216" s="1"/>
       <c r="X216" s="1"/>
     </row>
-    <row r="217" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>637</v>
       </c>
@@ -19623,7 +19629,7 @@
       <c r="W217" s="1"/>
       <c r="X217" s="1"/>
     </row>
-    <row r="218" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>637</v>
       </c>
@@ -19681,7 +19687,7 @@
       <c r="W218" s="1"/>
       <c r="X218" s="1"/>
     </row>
-    <row r="219" spans="1:24" ht="120" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:24" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>637</v>
       </c>
@@ -19739,7 +19745,7 @@
       <c r="W219" s="1"/>
       <c r="X219" s="1"/>
     </row>
-    <row r="220" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>637</v>
       </c>
@@ -19797,7 +19803,7 @@
       <c r="W220" s="1"/>
       <c r="X220" s="1"/>
     </row>
-    <row r="221" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>637</v>
       </c>
@@ -19855,7 +19861,7 @@
       <c r="W221" s="1"/>
       <c r="X221" s="1"/>
     </row>
-    <row r="222" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>637</v>
       </c>
@@ -19913,7 +19919,7 @@
       <c r="W222" s="1"/>
       <c r="X222" s="1"/>
     </row>
-    <row r="223" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>637</v>
       </c>
@@ -19971,7 +19977,7 @@
       <c r="W223" s="1"/>
       <c r="X223" s="1"/>
     </row>
-    <row r="224" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>637</v>
       </c>
@@ -20029,7 +20035,7 @@
       <c r="W224" s="1"/>
       <c r="X224" s="1"/>
     </row>
-    <row r="225" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>637</v>
       </c>
@@ -20087,7 +20093,7 @@
       <c r="W225" s="1"/>
       <c r="X225" s="1"/>
     </row>
-    <row r="226" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>637</v>
       </c>
@@ -20145,7 +20151,7 @@
       <c r="W226" s="1"/>
       <c r="X226" s="1"/>
     </row>
-    <row r="227" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>637</v>
       </c>
@@ -20203,7 +20209,7 @@
       <c r="W227" s="1"/>
       <c r="X227" s="1"/>
     </row>
-    <row r="228" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>637</v>
       </c>
@@ -20331,7 +20337,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="230" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>637</v>
       </c>
@@ -20389,7 +20395,7 @@
       <c r="W230" s="1"/>
       <c r="X230" s="1"/>
     </row>
-    <row r="231" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>637</v>
       </c>
@@ -20447,7 +20453,7 @@
       <c r="W231" s="1"/>
       <c r="X231" s="1"/>
     </row>
-    <row r="232" spans="1:24" ht="120" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:24" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>637</v>
       </c>
@@ -20505,7 +20511,7 @@
       <c r="W232" s="1"/>
       <c r="X232" s="1"/>
     </row>
-    <row r="233" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>637</v>
       </c>
@@ -20563,7 +20569,7 @@
       <c r="W233" s="1"/>
       <c r="X233" s="1"/>
     </row>
-    <row r="234" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>637</v>
       </c>
@@ -20621,7 +20627,7 @@
       <c r="W234" s="1"/>
       <c r="X234" s="1"/>
     </row>
-    <row r="235" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>637</v>
       </c>
@@ -20679,7 +20685,7 @@
       <c r="W235" s="1"/>
       <c r="X235" s="1"/>
     </row>
-    <row r="236" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>637</v>
       </c>
@@ -20737,7 +20743,7 @@
       <c r="W236" s="1"/>
       <c r="X236" s="1"/>
     </row>
-    <row r="237" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>637</v>
       </c>
@@ -20795,7 +20801,7 @@
       <c r="W237" s="1"/>
       <c r="X237" s="1"/>
     </row>
-    <row r="238" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>637</v>
       </c>
@@ -20853,7 +20859,7 @@
       <c r="W238" s="1"/>
       <c r="X238" s="1"/>
     </row>
-    <row r="239" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>637</v>
       </c>
@@ -20911,7 +20917,7 @@
       <c r="W239" s="1"/>
       <c r="X239" s="1"/>
     </row>
-    <row r="240" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>637</v>
       </c>
@@ -20969,7 +20975,7 @@
       <c r="W240" s="1"/>
       <c r="X240" s="1"/>
     </row>
-    <row r="241" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>637</v>
       </c>
@@ -21027,7 +21033,7 @@
       <c r="W241" s="1"/>
       <c r="X241" s="1"/>
     </row>
-    <row r="242" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>637</v>
       </c>
@@ -21085,7 +21091,7 @@
       <c r="W242" s="1"/>
       <c r="X242" s="1"/>
     </row>
-    <row r="243" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>637</v>
       </c>
@@ -21143,7 +21149,7 @@
       <c r="W243" s="1"/>
       <c r="X243" s="1"/>
     </row>
-    <row r="244" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>637</v>
       </c>
@@ -21201,7 +21207,7 @@
       <c r="W244" s="1"/>
       <c r="X244" s="1"/>
     </row>
-    <row r="245" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>637</v>
       </c>
@@ -21259,7 +21265,7 @@
       <c r="W245" s="1"/>
       <c r="X245" s="1"/>
     </row>
-    <row r="246" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>637</v>
       </c>
@@ -21317,7 +21323,7 @@
       <c r="W246" s="1"/>
       <c r="X246" s="1"/>
     </row>
-    <row r="247" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>637</v>
       </c>
@@ -21375,7 +21381,7 @@
       <c r="W247" s="1"/>
       <c r="X247" s="1"/>
     </row>
-    <row r="248" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>637</v>
       </c>
@@ -21433,7 +21439,7 @@
       <c r="W248" s="1"/>
       <c r="X248" s="1"/>
     </row>
-    <row r="249" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>637</v>
       </c>
@@ -21491,7 +21497,7 @@
       <c r="W249" s="1"/>
       <c r="X249" s="1"/>
     </row>
-    <row r="250" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:24" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>637</v>
       </c>
@@ -21549,7 +21555,7 @@
       <c r="W250" s="1"/>
       <c r="X250" s="1"/>
     </row>
-    <row r="251" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:24" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>637</v>
       </c>
@@ -21607,7 +21613,7 @@
       <c r="W251" s="1"/>
       <c r="X251" s="1"/>
     </row>
-    <row r="252" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:24" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>637</v>
       </c>
@@ -21665,7 +21671,7 @@
       <c r="W252" s="1"/>
       <c r="X252" s="1"/>
     </row>
-    <row r="253" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>637</v>
       </c>
@@ -21723,7 +21729,7 @@
       <c r="W253" s="1"/>
       <c r="X253" s="1"/>
     </row>
-    <row r="254" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>1786</v>
       </c>
@@ -21783,6 +21789,16 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:X254" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Computer Science"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A102:X149">
       <sortCondition ref="B1:B254"/>
     </sortState>

</xml_diff>